<commit_message>
app cleaner up & calculations updated
</commit_message>
<xml_diff>
--- a/public/formula.xlsx
+++ b/public/formula.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28605"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sangforltd-my.sharepoint.com/personal/akarsh_jain_sangfor_com/Documents/Sangfor Access Secure Collaterals/Sales and Ordering Guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46B2CF5B-C490-42B6-8146-D59BEA225E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{187293EE-8507-4B20-8B27-AB007DC77401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-700" yWindow="-20700" windowWidth="29600" windowHeight="19760" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-700" yWindow="-20700" windowWidth="29600" windowHeight="19760" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SASE ROI - Original" sheetId="1" r:id="rId1"/>
     <sheet name="SASE ROI - to USE" sheetId="4" r:id="rId2"/>
-    <sheet name="Lists" sheetId="2" r:id="rId3"/>
-    <sheet name="formula" sheetId="6" r:id="rId4"/>
+    <sheet name="formula" sheetId="6" r:id="rId3"/>
+    <sheet name="Lists" sheetId="2" r:id="rId4"/>
     <sheet name="References" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="213">
   <si>
     <t>ROI Calculator</t>
   </si>
@@ -545,6 +545,66 @@
     <t>ROI Calculator - to USE</t>
   </si>
   <si>
+    <t>Security and Networking Org Efficiency Gain</t>
+  </si>
+  <si>
+    <t>security team per employee</t>
+  </si>
+  <si>
+    <t>avg Time Spend on Administration</t>
+  </si>
+  <si>
+    <t>efficiency gains due to Access Secure</t>
+  </si>
+  <si>
+    <t>time tracking and responding to security</t>
+  </si>
+  <si>
+    <t>Size of the Networking Org</t>
+  </si>
+  <si>
+    <t>time spend on Administration</t>
+  </si>
+  <si>
+    <t>end users productivity impacted</t>
+  </si>
+  <si>
+    <t>productivity improvement</t>
+  </si>
+  <si>
+    <t>Average number of security</t>
+  </si>
+  <si>
+    <t>Average cost of data breach</t>
+  </si>
+  <si>
+    <t>Reduced likelihood of a breach</t>
+  </si>
+  <si>
+    <t>Security and Networking Infra Cost Reduction</t>
+  </si>
+  <si>
+    <t>number of employee cost</t>
+  </si>
+  <si>
+    <t>number of remote sites</t>
+  </si>
+  <si>
+    <t>DCs</t>
+  </si>
+  <si>
+    <t>Percentage of savings from vendor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of time spent for ongoing management </t>
+  </si>
+  <si>
+    <t>Cost of SASE Connector</t>
+  </si>
+  <si>
+    <t>Cost of Cross Border Traffic Acceleration</t>
+  </si>
+  <si>
     <t>Country</t>
   </si>
   <si>
@@ -585,30 +645,6 @@
   </si>
   <si>
     <t>UAE</t>
-  </si>
-  <si>
-    <t>security team per employee</t>
-  </si>
-  <si>
-    <t>Industry Trends</t>
-  </si>
-  <si>
-    <t>efficiency gains due to Access Secure</t>
-  </si>
-  <si>
-    <t>time tracking and responding to security</t>
-  </si>
-  <si>
-    <t>Size of the Networking Org</t>
-  </si>
-  <si>
-    <t>time spend on Administration</t>
-  </si>
-  <si>
-    <t>end users productivity impacted</t>
-  </si>
-  <si>
-    <t>productivity improvement</t>
   </si>
   <si>
     <t>Original Calculator File</t>
@@ -660,7 +696,7 @@
     <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.0_);[Red]\(&quot;$&quot;#,##0.0\)"/>
     <numFmt numFmtId="170" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,6 +789,19 @@
       <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -984,7 +1033,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1054,6 +1103,11 @@
     </xf>
     <xf numFmtId="168" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1099,9 +1153,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3321,7 +3372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S96"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="119" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A77" zoomScale="119" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -3659,37 +3710,37 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="13.7" customHeight="1">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
     </row>
     <row r="17" spans="1:10" ht="45.6" customHeight="1">
-      <c r="A17" s="59"/>
-      <c r="B17" s="62" t="s">
+      <c r="A17" s="64"/>
+      <c r="B17" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
     </row>
     <row r="18" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A18" s="59"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="18" t="s">
         <v>33</v>
       </c>
@@ -3705,15 +3756,15 @@
       <c r="F18" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="64" t="s">
+      <c r="G18" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
     </row>
     <row r="19" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A19" s="59"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="13" t="s">
         <v>36</v>
       </c>
@@ -3732,15 +3783,15 @@
         <f>D19</f>
         <v>4</v>
       </c>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A20" s="59"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="13" t="s">
         <v>39</v>
       </c>
@@ -3756,15 +3807,15 @@
       <c r="F20" s="23">
         <v>0.6</v>
       </c>
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
     </row>
     <row r="21" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A21" s="59"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="13" t="s">
         <v>42</v>
       </c>
@@ -3780,15 +3831,15 @@
       <c r="F21" s="23">
         <v>0.65</v>
       </c>
-      <c r="G21" s="58" t="s">
+      <c r="G21" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="59"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="19" t="s">
         <v>45</v>
       </c>
@@ -3807,13 +3858,13 @@
         <f>ROUNDUP(F19*F20*F21,0)</f>
         <v>2</v>
       </c>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="59"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="13" t="s">
         <v>47</v>
       </c>
@@ -3829,15 +3880,15 @@
       <c r="F23" s="23">
         <v>0.15</v>
       </c>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
     </row>
     <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="59"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="13" t="s">
         <v>49</v>
       </c>
@@ -3853,15 +3904,15 @@
       <c r="F24" s="23">
         <v>0.65</v>
       </c>
-      <c r="G24" s="58" t="s">
+      <c r="G24" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
     </row>
     <row r="25" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A25" s="59"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="19" t="s">
         <v>50</v>
       </c>
@@ -3880,13 +3931,13 @@
         <f>ROUNDUP(F19*F23*F24,0)</f>
         <v>1</v>
       </c>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
     </row>
     <row r="26" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A26" s="59"/>
+      <c r="A26" s="64"/>
       <c r="B26" s="13" t="s">
         <v>52</v>
       </c>
@@ -3905,15 +3956,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$F$12,2,FALSE)</f>
         <v>50280</v>
       </c>
-      <c r="G26" s="58" t="s">
+      <c r="G26" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
     </row>
     <row r="27" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A27" s="59"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="20" t="s">
         <v>55</v>
       </c>
@@ -3932,27 +3983,27 @@
         <f>(F22+F25)*F26</f>
         <v>150840</v>
       </c>
-      <c r="G27" s="58" t="s">
+      <c r="G27" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
     </row>
     <row r="28" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A28" s="59"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="67"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="72"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="59"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="13" t="s">
         <v>58</v>
       </c>
@@ -3971,15 +4022,15 @@
         <f>D29</f>
         <v>3</v>
       </c>
-      <c r="G29" s="58" t="s">
+      <c r="G29" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="59"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="13" t="s">
         <v>61</v>
       </c>
@@ -3995,15 +4046,15 @@
       <c r="F30" s="23">
         <v>0.33</v>
       </c>
-      <c r="G30" s="58" t="s">
+      <c r="G30" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
     </row>
     <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="59"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="13" t="s">
         <v>63</v>
       </c>
@@ -4019,15 +4070,15 @@
       <c r="F31" s="23">
         <v>0.65</v>
       </c>
-      <c r="G31" s="58" t="s">
+      <c r="G31" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A32" s="59"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
@@ -4046,13 +4097,13 @@
         <f>ROUNDUP(F29*F30*F31,0)</f>
         <v>1</v>
       </c>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A33" s="59"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="13" t="s">
         <v>66</v>
       </c>
@@ -4071,15 +4122,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$G$12,3,FALSE)</f>
         <v>46862</v>
       </c>
-      <c r="G33" s="58" t="s">
+      <c r="G33" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
     </row>
     <row r="34" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A34" s="59"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="16" t="s">
         <v>68</v>
       </c>
@@ -4098,27 +4149,27 @@
         <f>F33*F32</f>
         <v>46862</v>
       </c>
-      <c r="G34" s="58" t="s">
+      <c r="G34" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
     </row>
     <row r="35" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A35" s="59"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
     </row>
     <row r="36" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A36" s="59"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="13" t="s">
         <v>70</v>
       </c>
@@ -4134,15 +4185,15 @@
       <c r="F36" s="4">
         <v>0.25</v>
       </c>
-      <c r="G36" s="58" t="s">
+      <c r="G36" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
     </row>
     <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="59"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="13" t="s">
         <v>73</v>
       </c>
@@ -4158,15 +4209,15 @@
       <c r="F37" s="4">
         <v>0.1</v>
       </c>
-      <c r="G37" s="57" t="s">
+      <c r="G37" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="H37" s="57"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
     </row>
     <row r="38" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A38" s="59"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="16" t="s">
         <v>76</v>
       </c>
@@ -4183,43 +4234,43 @@
         <f>(F27+F34)*(1-F36)*(1-F37)</f>
         <v>133448.85</v>
       </c>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="58"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
     </row>
     <row r="40" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A40" s="59" t="s">
+      <c r="A40" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="B40" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="61"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="61"/>
-      <c r="J40" s="61"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="66"/>
     </row>
     <row r="41" spans="1:10" ht="45" customHeight="1">
-      <c r="A41" s="59"/>
-      <c r="B41" s="62" t="s">
+      <c r="A41" s="64"/>
+      <c r="B41" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
-      <c r="I41" s="63"/>
-      <c r="J41" s="63"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="68"/>
+      <c r="J41" s="68"/>
     </row>
     <row r="42" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A42" s="59"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="18" t="s">
         <v>33</v>
       </c>
@@ -4235,15 +4286,15 @@
       <c r="F42" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="64" t="s">
+      <c r="G42" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H42" s="64"/>
-      <c r="I42" s="64"/>
-      <c r="J42" s="64"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="69"/>
     </row>
     <row r="43" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A43" s="59"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="13" t="s">
         <v>79</v>
       </c>
@@ -4262,13 +4313,13 @@
         <f>D3</f>
         <v>5000</v>
       </c>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
     </row>
     <row r="44" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A44" s="59"/>
+      <c r="A44" s="64"/>
       <c r="B44" s="13" t="s">
         <v>81</v>
       </c>
@@ -4287,13 +4338,13 @@
         <f>D4</f>
         <v>0.5</v>
       </c>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
     </row>
     <row r="45" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A45" s="59"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="13" t="s">
         <v>83</v>
       </c>
@@ -4309,15 +4360,15 @@
       <c r="F45" s="4">
         <v>0.2</v>
       </c>
-      <c r="G45" s="58" t="s">
+      <c r="G45" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
     </row>
     <row r="46" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A46" s="59"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="10" t="s">
         <v>86</v>
       </c>
@@ -4336,13 +4387,13 @@
         <f>F43*F44*F45</f>
         <v>500</v>
       </c>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
+      <c r="G46" s="63"/>
+      <c r="H46" s="63"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
     </row>
     <row r="47" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A47" s="59"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="13" t="s">
         <v>88</v>
       </c>
@@ -4358,15 +4409,15 @@
       <c r="F47" s="23">
         <v>0.08</v>
       </c>
-      <c r="G47" s="58" t="s">
+      <c r="G47" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
     </row>
     <row r="48" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A48" s="59"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="10" t="s">
         <v>90</v>
       </c>
@@ -4385,13 +4436,13 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="63"/>
+      <c r="J48" s="63"/>
     </row>
     <row r="49" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A49" s="59"/>
+      <c r="A49" s="64"/>
       <c r="B49" s="13" t="s">
         <v>92</v>
       </c>
@@ -4410,15 +4461,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$H$12,4,FALSE)</f>
         <v>41000</v>
       </c>
-      <c r="G49" s="58" t="s">
+      <c r="G49" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="63"/>
+      <c r="J49" s="63"/>
     </row>
     <row r="50" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A50" s="59"/>
+      <c r="A50" s="64"/>
       <c r="B50" s="16" t="s">
         <v>95</v>
       </c>
@@ -4437,27 +4488,27 @@
         <f>F48*F49</f>
         <v>1640000</v>
       </c>
-      <c r="G50" s="58" t="s">
+      <c r="G50" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="58"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="63"/>
+      <c r="J50" s="63"/>
     </row>
     <row r="51" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A51" s="59"/>
-      <c r="B51" s="66"/>
-      <c r="C51" s="66"/>
-      <c r="D51" s="66"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="66"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="66"/>
-      <c r="I51" s="66"/>
-      <c r="J51" s="67"/>
+      <c r="A51" s="64"/>
+      <c r="B51" s="71"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="71"/>
+      <c r="G51" s="71"/>
+      <c r="H51" s="71"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="72"/>
     </row>
     <row r="52" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A52" s="59"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="13" t="s">
         <v>97</v>
       </c>
@@ -4473,15 +4524,15 @@
       <c r="F52" s="4">
         <v>0.25</v>
       </c>
-      <c r="G52" s="58" t="s">
+      <c r="G52" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
-      <c r="J52" s="58"/>
+      <c r="H52" s="63"/>
+      <c r="I52" s="63"/>
+      <c r="J52" s="63"/>
     </row>
     <row r="53" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A53" s="59"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="13" t="s">
         <v>99</v>
       </c>
@@ -4497,15 +4548,15 @@
       <c r="F53" s="4">
         <v>0.1</v>
       </c>
-      <c r="G53" s="57" t="s">
+      <c r="G53" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="H53" s="57"/>
-      <c r="I53" s="57"/>
-      <c r="J53" s="57"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="62"/>
     </row>
     <row r="54" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A54" s="59"/>
+      <c r="A54" s="64"/>
       <c r="B54" s="16" t="s">
         <v>100</v>
       </c>
@@ -4522,43 +4573,43 @@
         <f>F50*(1-F52)*(1-F53)</f>
         <v>1107000</v>
       </c>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
     </row>
     <row r="56" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="60" t="s">
+      <c r="B56" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="61"/>
-      <c r="D56" s="61"/>
-      <c r="E56" s="61"/>
-      <c r="F56" s="61"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="61"/>
-      <c r="I56" s="61"/>
-      <c r="J56" s="61"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="66"/>
+      <c r="F56" s="66"/>
+      <c r="G56" s="66"/>
+      <c r="H56" s="66"/>
+      <c r="I56" s="66"/>
+      <c r="J56" s="66"/>
     </row>
     <row r="57" spans="1:10" ht="49.35" customHeight="1">
-      <c r="A57" s="59"/>
-      <c r="B57" s="62" t="s">
+      <c r="A57" s="64"/>
+      <c r="B57" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="63"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="63"/>
-      <c r="F57" s="63"/>
-      <c r="G57" s="63"/>
-      <c r="H57" s="63"/>
-      <c r="I57" s="63"/>
-      <c r="J57" s="63"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="68"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="68"/>
+      <c r="J57" s="68"/>
     </row>
     <row r="58" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A58" s="59"/>
+      <c r="A58" s="64"/>
       <c r="B58" s="18" t="s">
         <v>33</v>
       </c>
@@ -4574,15 +4625,15 @@
       <c r="F58" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G58" s="64" t="s">
+      <c r="G58" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H58" s="64"/>
-      <c r="I58" s="64"/>
-      <c r="J58" s="64"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="69"/>
+      <c r="J58" s="69"/>
     </row>
     <row r="59" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A59" s="59"/>
+      <c r="A59" s="64"/>
       <c r="B59" s="13" t="s">
         <v>103</v>
       </c>
@@ -4600,15 +4651,15 @@
         <f>D59</f>
         <v>3.2</v>
       </c>
-      <c r="G59" s="58" t="s">
+      <c r="G59" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
-      <c r="J59" s="58"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="63"/>
+      <c r="J59" s="63"/>
     </row>
     <row r="60" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A60" s="59"/>
+      <c r="A60" s="64"/>
       <c r="B60" s="13" t="s">
         <v>106</v>
       </c>
@@ -4627,13 +4678,13 @@
         <f>E60</f>
         <v>5000</v>
       </c>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="58"/>
-      <c r="J60" s="58"/>
+      <c r="G60" s="63"/>
+      <c r="H60" s="63"/>
+      <c r="I60" s="63"/>
+      <c r="J60" s="63"/>
     </row>
     <row r="61" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A61" s="59"/>
+      <c r="A61" s="64"/>
       <c r="B61" s="13" t="s">
         <v>107</v>
       </c>
@@ -4652,13 +4703,13 @@
         <f>E61</f>
         <v>0.5</v>
       </c>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
-      <c r="J61" s="58"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="63"/>
+      <c r="I61" s="63"/>
+      <c r="J61" s="63"/>
     </row>
     <row r="62" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A62" s="59"/>
+      <c r="A62" s="64"/>
       <c r="B62" s="13" t="s">
         <v>108</v>
       </c>
@@ -4674,15 +4725,15 @@
       <c r="F62" s="5">
         <v>53</v>
       </c>
-      <c r="G62" s="65" t="s">
+      <c r="G62" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="H62" s="65"/>
-      <c r="I62" s="65"/>
-      <c r="J62" s="65"/>
+      <c r="H62" s="70"/>
+      <c r="I62" s="70"/>
+      <c r="J62" s="70"/>
     </row>
     <row r="63" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A63" s="59"/>
+      <c r="A63" s="64"/>
       <c r="B63" s="10" t="s">
         <v>111</v>
       </c>
@@ -4701,13 +4752,13 @@
         <f>F59*F60*F61*F62</f>
         <v>424000</v>
       </c>
-      <c r="G63" s="58"/>
-      <c r="H63" s="58"/>
-      <c r="I63" s="58"/>
-      <c r="J63" s="58"/>
+      <c r="G63" s="63"/>
+      <c r="H63" s="63"/>
+      <c r="I63" s="63"/>
+      <c r="J63" s="63"/>
     </row>
     <row r="64" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A64" s="59"/>
+      <c r="A64" s="64"/>
       <c r="B64" s="13" t="s">
         <v>113</v>
       </c>
@@ -4723,15 +4774,15 @@
       <c r="F64" s="4">
         <v>0.75</v>
       </c>
-      <c r="G64" s="58" t="s">
+      <c r="G64" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H64" s="58"/>
-      <c r="I64" s="58"/>
-      <c r="J64" s="58"/>
+      <c r="H64" s="63"/>
+      <c r="I64" s="63"/>
+      <c r="J64" s="63"/>
     </row>
     <row r="65" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A65" s="59"/>
+      <c r="A65" s="64"/>
       <c r="B65" s="16" t="s">
         <v>115</v>
       </c>
@@ -4750,25 +4801,25 @@
         <f t="shared" si="4"/>
         <v>318000</v>
       </c>
-      <c r="G65" s="53"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="54"/>
-      <c r="J65" s="55"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="59"/>
+      <c r="J65" s="60"/>
     </row>
     <row r="66" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A66" s="59"/>
-      <c r="B66" s="56"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="56"/>
-      <c r="I66" s="56"/>
-      <c r="J66" s="56"/>
+      <c r="A66" s="64"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="61"/>
+      <c r="G66" s="61"/>
+      <c r="H66" s="61"/>
+      <c r="I66" s="61"/>
+      <c r="J66" s="61"/>
     </row>
     <row r="67" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A67" s="59"/>
+      <c r="A67" s="64"/>
       <c r="B67" s="13" t="s">
         <v>117</v>
       </c>
@@ -4784,15 +4835,15 @@
       <c r="F67" s="4">
         <v>0.25</v>
       </c>
-      <c r="G67" s="57" t="s">
+      <c r="G67" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="H67" s="57"/>
-      <c r="I67" s="57"/>
-      <c r="J67" s="57"/>
+      <c r="H67" s="62"/>
+      <c r="I67" s="62"/>
+      <c r="J67" s="62"/>
     </row>
     <row r="68" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A68" s="59"/>
+      <c r="A68" s="64"/>
       <c r="B68" s="16" t="s">
         <v>118</v>
       </c>
@@ -4809,43 +4860,43 @@
         <f>F65*(1-F67)</f>
         <v>238500</v>
       </c>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="58"/>
-      <c r="J68" s="58"/>
+      <c r="G68" s="63"/>
+      <c r="H68" s="63"/>
+      <c r="I68" s="63"/>
+      <c r="J68" s="63"/>
     </row>
     <row r="70" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A70" s="59" t="s">
+      <c r="A70" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="B70" s="60" t="s">
+      <c r="B70" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C70" s="61"/>
-      <c r="D70" s="61"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="61"/>
-      <c r="G70" s="61"/>
-      <c r="H70" s="61"/>
-      <c r="I70" s="61"/>
-      <c r="J70" s="61"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
+      <c r="H70" s="66"/>
+      <c r="I70" s="66"/>
+      <c r="J70" s="66"/>
     </row>
     <row r="71" spans="1:10" ht="41.45" customHeight="1">
-      <c r="A71" s="59"/>
-      <c r="B71" s="62" t="s">
+      <c r="A71" s="64"/>
+      <c r="B71" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="63"/>
-      <c r="D71" s="63"/>
-      <c r="E71" s="63"/>
-      <c r="F71" s="63"/>
-      <c r="G71" s="63"/>
-      <c r="H71" s="63"/>
-      <c r="I71" s="63"/>
-      <c r="J71" s="63"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="68"/>
+      <c r="F71" s="68"/>
+      <c r="G71" s="68"/>
+      <c r="H71" s="68"/>
+      <c r="I71" s="68"/>
+      <c r="J71" s="68"/>
     </row>
     <row r="72" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A72" s="59"/>
+      <c r="A72" s="64"/>
       <c r="B72" s="18" t="s">
         <v>33</v>
       </c>
@@ -4861,15 +4912,15 @@
       <c r="F72" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G72" s="64" t="s">
+      <c r="G72" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H72" s="64"/>
-      <c r="I72" s="64"/>
-      <c r="J72" s="64"/>
+      <c r="H72" s="69"/>
+      <c r="I72" s="69"/>
+      <c r="J72" s="69"/>
     </row>
     <row r="73" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A73" s="59"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="13" t="s">
         <v>121</v>
       </c>
@@ -4888,15 +4939,15 @@
         <f>E73</f>
         <v>175000</v>
       </c>
-      <c r="G73" s="65" t="s">
+      <c r="G73" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="H73" s="65"/>
-      <c r="I73" s="65"/>
-      <c r="J73" s="65"/>
+      <c r="H73" s="70"/>
+      <c r="I73" s="70"/>
+      <c r="J73" s="70"/>
     </row>
     <row r="74" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A74" s="59"/>
+      <c r="A74" s="64"/>
       <c r="B74" s="13" t="s">
         <v>124</v>
       </c>
@@ -4912,15 +4963,15 @@
       <c r="F74" s="28">
         <v>0.3</v>
       </c>
-      <c r="G74" s="58" t="s">
+      <c r="G74" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="H74" s="58"/>
-      <c r="I74" s="58"/>
-      <c r="J74" s="58"/>
+      <c r="H74" s="63"/>
+      <c r="I74" s="63"/>
+      <c r="J74" s="63"/>
     </row>
     <row r="75" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A75" s="59"/>
+      <c r="A75" s="64"/>
       <c r="B75" s="13" t="s">
         <v>127</v>
       </c>
@@ -4939,15 +4990,15 @@
         <f>IF($D$5="Yes",$G$4*36000,0)</f>
         <v>72000</v>
       </c>
-      <c r="G75" s="58" t="s">
+      <c r="G75" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="H75" s="58"/>
-      <c r="I75" s="58"/>
-      <c r="J75" s="58"/>
+      <c r="H75" s="63"/>
+      <c r="I75" s="63"/>
+      <c r="J75" s="63"/>
     </row>
     <row r="76" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A76" s="59"/>
+      <c r="A76" s="64"/>
       <c r="B76" s="13" t="s">
         <v>130</v>
       </c>
@@ -4966,13 +5017,13 @@
         <f>(F73*F74)+F75</f>
         <v>124500</v>
       </c>
-      <c r="G76" s="58"/>
-      <c r="H76" s="58"/>
-      <c r="I76" s="58"/>
-      <c r="J76" s="58"/>
+      <c r="G76" s="63"/>
+      <c r="H76" s="63"/>
+      <c r="I76" s="63"/>
+      <c r="J76" s="63"/>
     </row>
     <row r="77" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A77" s="59"/>
+      <c r="A77" s="64"/>
       <c r="B77" s="13" t="s">
         <v>132</v>
       </c>
@@ -4988,13 +5039,13 @@
       <c r="F77" s="28">
         <v>0.1</v>
       </c>
-      <c r="G77" s="65"/>
-      <c r="H77" s="65"/>
-      <c r="I77" s="65"/>
-      <c r="J77" s="65"/>
+      <c r="G77" s="70"/>
+      <c r="H77" s="70"/>
+      <c r="I77" s="70"/>
+      <c r="J77" s="70"/>
     </row>
     <row r="78" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A78" s="59"/>
+      <c r="A78" s="64"/>
       <c r="B78" s="16" t="s">
         <v>130</v>
       </c>
@@ -5011,43 +5062,43 @@
         <f>F76*(1-F77)</f>
         <v>112050</v>
       </c>
-      <c r="G78" s="53"/>
-      <c r="H78" s="54"/>
-      <c r="I78" s="54"/>
-      <c r="J78" s="55"/>
+      <c r="G78" s="58"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="59"/>
+      <c r="J78" s="60"/>
     </row>
     <row r="80" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A80" s="59" t="s">
+      <c r="A80" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="B80" s="60" t="s">
+      <c r="B80" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="C80" s="61"/>
-      <c r="D80" s="61"/>
-      <c r="E80" s="61"/>
-      <c r="F80" s="61"/>
-      <c r="G80" s="61"/>
-      <c r="H80" s="61"/>
-      <c r="I80" s="61"/>
-      <c r="J80" s="61"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="66"/>
+      <c r="E80" s="66"/>
+      <c r="F80" s="66"/>
+      <c r="G80" s="66"/>
+      <c r="H80" s="66"/>
+      <c r="I80" s="66"/>
+      <c r="J80" s="66"/>
     </row>
     <row r="81" spans="1:10" ht="78" customHeight="1">
-      <c r="A81" s="59"/>
-      <c r="B81" s="62" t="s">
+      <c r="A81" s="64"/>
+      <c r="B81" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="C81" s="63"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
-      <c r="F81" s="63"/>
-      <c r="G81" s="63"/>
-      <c r="H81" s="63"/>
-      <c r="I81" s="63"/>
-      <c r="J81" s="63"/>
+      <c r="C81" s="68"/>
+      <c r="D81" s="68"/>
+      <c r="E81" s="68"/>
+      <c r="F81" s="68"/>
+      <c r="G81" s="68"/>
+      <c r="H81" s="68"/>
+      <c r="I81" s="68"/>
+      <c r="J81" s="68"/>
     </row>
     <row r="82" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A82" s="59"/>
+      <c r="A82" s="64"/>
       <c r="B82" s="18" t="s">
         <v>33</v>
       </c>
@@ -5063,15 +5114,15 @@
       <c r="F82" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G82" s="64" t="s">
+      <c r="G82" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H82" s="64"/>
-      <c r="I82" s="64"/>
-      <c r="J82" s="64"/>
+      <c r="H82" s="69"/>
+      <c r="I82" s="69"/>
+      <c r="J82" s="69"/>
     </row>
     <row r="83" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A83" s="59"/>
+      <c r="A83" s="64"/>
       <c r="B83" s="13" t="s">
         <v>137</v>
       </c>
@@ -5090,15 +5141,15 @@
         <f>ROUNDUP(D3/2000,0)</f>
         <v>3</v>
       </c>
-      <c r="G83" s="65" t="s">
+      <c r="G83" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="H83" s="65"/>
-      <c r="I83" s="65"/>
-      <c r="J83" s="65"/>
+      <c r="H83" s="70"/>
+      <c r="I83" s="70"/>
+      <c r="J83" s="70"/>
     </row>
     <row r="84" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A84" s="59"/>
+      <c r="A84" s="64"/>
       <c r="B84" s="13" t="s">
         <v>140</v>
       </c>
@@ -5114,15 +5165,15 @@
       <c r="F84" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G84" s="53" t="s">
+      <c r="G84" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="H84" s="54"/>
-      <c r="I84" s="54"/>
-      <c r="J84" s="55"/>
+      <c r="H84" s="59"/>
+      <c r="I84" s="59"/>
+      <c r="J84" s="60"/>
     </row>
     <row r="85" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A85" s="59"/>
+      <c r="A85" s="64"/>
       <c r="B85" s="13" t="s">
         <v>143</v>
       </c>
@@ -5138,15 +5189,15 @@
       <c r="F85" s="23">
         <v>0.05</v>
       </c>
-      <c r="G85" s="53" t="s">
+      <c r="G85" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="H85" s="54"/>
-      <c r="I85" s="54"/>
-      <c r="J85" s="55"/>
+      <c r="H85" s="59"/>
+      <c r="I85" s="59"/>
+      <c r="J85" s="60"/>
     </row>
     <row r="86" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A86" s="59"/>
+      <c r="A86" s="64"/>
       <c r="B86" s="13" t="s">
         <v>146</v>
       </c>
@@ -5165,15 +5216,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$F$12,2,FALSE)</f>
         <v>50280</v>
       </c>
-      <c r="G86" s="58" t="s">
+      <c r="G86" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="H86" s="58"/>
-      <c r="I86" s="58"/>
-      <c r="J86" s="58"/>
+      <c r="H86" s="63"/>
+      <c r="I86" s="63"/>
+      <c r="J86" s="63"/>
     </row>
     <row r="87" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A87" s="59"/>
+      <c r="A87" s="64"/>
       <c r="B87" s="10" t="s">
         <v>148</v>
       </c>
@@ -5192,13 +5243,13 @@
         <f>F83*(F84+F85)*F86</f>
         <v>18100.800000000003</v>
       </c>
-      <c r="G87" s="58"/>
-      <c r="H87" s="58"/>
-      <c r="I87" s="58"/>
-      <c r="J87" s="58"/>
+      <c r="G87" s="63"/>
+      <c r="H87" s="63"/>
+      <c r="I87" s="63"/>
+      <c r="J87" s="63"/>
     </row>
     <row r="88" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A88" s="59"/>
+      <c r="A88" s="64"/>
       <c r="B88" s="13" t="s">
         <v>150</v>
       </c>
@@ -5214,15 +5265,15 @@
       <c r="F88" s="4">
         <v>0.02</v>
       </c>
-      <c r="G88" s="53" t="s">
+      <c r="G88" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="H88" s="54"/>
-      <c r="I88" s="54"/>
-      <c r="J88" s="55"/>
+      <c r="H88" s="59"/>
+      <c r="I88" s="59"/>
+      <c r="J88" s="60"/>
     </row>
     <row r="89" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A89" s="59"/>
+      <c r="A89" s="64"/>
       <c r="B89" s="10" t="s">
         <v>152</v>
       </c>
@@ -5241,13 +5292,13 @@
         <f>F83*(F86)*F88</f>
         <v>3016.8</v>
       </c>
-      <c r="G89" s="58"/>
-      <c r="H89" s="58"/>
-      <c r="I89" s="58"/>
-      <c r="J89" s="58"/>
+      <c r="G89" s="63"/>
+      <c r="H89" s="63"/>
+      <c r="I89" s="63"/>
+      <c r="J89" s="63"/>
     </row>
     <row r="90" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A90" s="59"/>
+      <c r="A90" s="64"/>
       <c r="B90" s="13" t="s">
         <v>154</v>
       </c>
@@ -5266,15 +5317,15 @@
         <f>$J$4*$D$3</f>
         <v>325000</v>
       </c>
-      <c r="G90" s="58" t="s">
+      <c r="G90" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="H90" s="58"/>
-      <c r="I90" s="58"/>
-      <c r="J90" s="58"/>
+      <c r="H90" s="63"/>
+      <c r="I90" s="63"/>
+      <c r="J90" s="63"/>
     </row>
     <row r="91" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A91" s="59"/>
+      <c r="A91" s="64"/>
       <c r="B91" s="13" t="s">
         <v>157</v>
       </c>
@@ -5293,15 +5344,15 @@
         <f t="shared" si="5"/>
         <v>1200</v>
       </c>
-      <c r="G91" s="53" t="s">
+      <c r="G91" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="H91" s="54"/>
-      <c r="I91" s="54"/>
-      <c r="J91" s="55"/>
+      <c r="H91" s="59"/>
+      <c r="I91" s="59"/>
+      <c r="J91" s="60"/>
     </row>
     <row r="92" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A92" s="59"/>
+      <c r="A92" s="64"/>
       <c r="B92" s="13" t="s">
         <v>160</v>
       </c>
@@ -5320,15 +5371,15 @@
         <f>IF($D$5="Yes",$G$4*4500,0)</f>
         <v>9000</v>
       </c>
-      <c r="G92" s="53" t="s">
+      <c r="G92" s="58" t="s">
         <v>162</v>
       </c>
-      <c r="H92" s="54"/>
-      <c r="I92" s="54"/>
-      <c r="J92" s="55"/>
+      <c r="H92" s="59"/>
+      <c r="I92" s="59"/>
+      <c r="J92" s="60"/>
     </row>
     <row r="93" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A93" s="59"/>
+      <c r="A93" s="64"/>
       <c r="B93" s="29" t="s">
         <v>163</v>
       </c>
@@ -5347,25 +5398,25 @@
         <f>SUM(F87,F89:F92)</f>
         <v>356317.6</v>
       </c>
-      <c r="G93" s="53"/>
-      <c r="H93" s="54"/>
-      <c r="I93" s="54"/>
-      <c r="J93" s="55"/>
+      <c r="G93" s="58"/>
+      <c r="H93" s="59"/>
+      <c r="I93" s="59"/>
+      <c r="J93" s="60"/>
     </row>
     <row r="94" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A94" s="59"/>
-      <c r="B94" s="56"/>
-      <c r="C94" s="56"/>
-      <c r="D94" s="56"/>
-      <c r="E94" s="56"/>
-      <c r="F94" s="56"/>
-      <c r="G94" s="56"/>
-      <c r="H94" s="56"/>
-      <c r="I94" s="56"/>
-      <c r="J94" s="56"/>
+      <c r="A94" s="64"/>
+      <c r="B94" s="61"/>
+      <c r="C94" s="61"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="61"/>
+      <c r="F94" s="61"/>
+      <c r="G94" s="61"/>
+      <c r="H94" s="61"/>
+      <c r="I94" s="61"/>
+      <c r="J94" s="61"/>
     </row>
     <row r="95" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A95" s="59"/>
+      <c r="A95" s="64"/>
       <c r="B95" s="13" t="s">
         <v>165</v>
       </c>
@@ -5381,13 +5432,13 @@
       <c r="F95" s="4">
         <v>0.05</v>
       </c>
-      <c r="G95" s="57"/>
-      <c r="H95" s="57"/>
-      <c r="I95" s="57"/>
-      <c r="J95" s="57"/>
+      <c r="G95" s="62"/>
+      <c r="H95" s="62"/>
+      <c r="I95" s="62"/>
+      <c r="J95" s="62"/>
     </row>
     <row r="96" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A96" s="59"/>
+      <c r="A96" s="64"/>
       <c r="B96" s="16"/>
       <c r="C96" s="16"/>
       <c r="D96" s="26">
@@ -5402,10 +5453,10 @@
         <f>F93*(1+F95)</f>
         <v>374133.48</v>
       </c>
-      <c r="G96" s="58"/>
-      <c r="H96" s="58"/>
-      <c r="I96" s="58"/>
-      <c r="J96" s="58"/>
+      <c r="G96" s="63"/>
+      <c r="H96" s="63"/>
+      <c r="I96" s="63"/>
+      <c r="J96" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="82">
@@ -5520,8 +5571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972358DD-1820-401E-852C-2CB83E566002}">
   <dimension ref="A1:S96"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" zoomScale="119" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView showGridLines="0" topLeftCell="A63" zoomScale="119" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73:J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.7" customHeight="1"/>
@@ -5860,37 +5911,37 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="13.7" customHeight="1">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
     </row>
     <row r="17" spans="1:10" ht="45.6" customHeight="1">
-      <c r="A17" s="59"/>
-      <c r="B17" s="62" t="s">
+      <c r="A17" s="64"/>
+      <c r="B17" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
     </row>
     <row r="18" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A18" s="59"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="18" t="s">
         <v>33</v>
       </c>
@@ -5906,15 +5957,15 @@
       <c r="F18" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="64" t="s">
+      <c r="G18" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
     </row>
     <row r="19" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A19" s="59"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="13" t="s">
         <v>36</v>
       </c>
@@ -5933,15 +5984,15 @@
         <f>D19</f>
         <v>4</v>
       </c>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A20" s="59"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="13" t="s">
         <v>39</v>
       </c>
@@ -5957,15 +6008,15 @@
       <c r="F20" s="23">
         <v>0.6</v>
       </c>
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
     </row>
     <row r="21" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A21" s="59"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="13" t="s">
         <v>42</v>
       </c>
@@ -5981,15 +6032,15 @@
       <c r="F21" s="23">
         <v>0.65</v>
       </c>
-      <c r="G21" s="58" t="s">
+      <c r="G21" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="59"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="19" t="s">
         <v>45</v>
       </c>
@@ -6008,13 +6059,13 @@
         <f>ROUNDUP(F19*F20*F21,0)</f>
         <v>2</v>
       </c>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="59"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="13" t="s">
         <v>47</v>
       </c>
@@ -6030,15 +6081,15 @@
       <c r="F23" s="23">
         <v>0.15</v>
       </c>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
     </row>
     <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="59"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="13" t="s">
         <v>49</v>
       </c>
@@ -6054,15 +6105,15 @@
       <c r="F24" s="23">
         <v>0.65</v>
       </c>
-      <c r="G24" s="58" t="s">
+      <c r="G24" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
     </row>
     <row r="25" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A25" s="59"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="19" t="s">
         <v>50</v>
       </c>
@@ -6081,13 +6132,13 @@
         <f>ROUNDUP(F19*F23*F24,0)</f>
         <v>1</v>
       </c>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
     </row>
     <row r="26" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A26" s="59"/>
+      <c r="A26" s="64"/>
       <c r="B26" s="13" t="s">
         <v>52</v>
       </c>
@@ -6106,15 +6157,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$F$12,2,FALSE)</f>
         <v>50280</v>
       </c>
-      <c r="G26" s="58" t="s">
+      <c r="G26" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
     </row>
     <row r="27" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A27" s="59"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="20" t="s">
         <v>55</v>
       </c>
@@ -6133,27 +6184,27 @@
         <f>(F22+F25)*F26</f>
         <v>150840</v>
       </c>
-      <c r="G27" s="58" t="s">
+      <c r="G27" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
     </row>
     <row r="28" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A28" s="59"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="67"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="72"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="59"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="13" t="s">
         <v>58</v>
       </c>
@@ -6172,15 +6223,15 @@
         <f>D29</f>
         <v>3</v>
       </c>
-      <c r="G29" s="58" t="s">
+      <c r="G29" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="59"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="13" t="s">
         <v>61</v>
       </c>
@@ -6196,15 +6247,15 @@
       <c r="F30" s="23">
         <v>0.33</v>
       </c>
-      <c r="G30" s="58" t="s">
+      <c r="G30" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
     </row>
     <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="59"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="13" t="s">
         <v>63</v>
       </c>
@@ -6220,15 +6271,15 @@
       <c r="F31" s="23">
         <v>0.65</v>
       </c>
-      <c r="G31" s="58" t="s">
+      <c r="G31" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A32" s="59"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
@@ -6247,13 +6298,13 @@
         <f>ROUNDUP(F29*F30*F31,0)</f>
         <v>1</v>
       </c>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A33" s="59"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="13" t="s">
         <v>66</v>
       </c>
@@ -6272,15 +6323,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$G$12,3,FALSE)</f>
         <v>46862</v>
       </c>
-      <c r="G33" s="58" t="s">
+      <c r="G33" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
     </row>
     <row r="34" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A34" s="59"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="16" t="s">
         <v>68</v>
       </c>
@@ -6299,27 +6350,27 @@
         <f>F33*F32</f>
         <v>46862</v>
       </c>
-      <c r="G34" s="58" t="s">
+      <c r="G34" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
     </row>
     <row r="35" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A35" s="59"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
     </row>
     <row r="36" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A36" s="59"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="13" t="s">
         <v>70</v>
       </c>
@@ -6335,15 +6386,15 @@
       <c r="F36" s="4">
         <v>0.25</v>
       </c>
-      <c r="G36" s="58" t="s">
+      <c r="G36" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
     </row>
     <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="59"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="13" t="s">
         <v>73</v>
       </c>
@@ -6359,15 +6410,15 @@
       <c r="F37" s="4">
         <v>0.1</v>
       </c>
-      <c r="G37" s="57" t="s">
+      <c r="G37" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="H37" s="57"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
     </row>
     <row r="38" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A38" s="59"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="16" t="s">
         <v>76</v>
       </c>
@@ -6384,43 +6435,43 @@
         <f>(F27+F34)*(1-F36)*(1-F37)</f>
         <v>133448.85</v>
       </c>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="58"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
     </row>
     <row r="40" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A40" s="59" t="s">
+      <c r="A40" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="B40" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="61"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="61"/>
-      <c r="J40" s="61"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="66"/>
     </row>
     <row r="41" spans="1:10" ht="45" customHeight="1">
-      <c r="A41" s="59"/>
-      <c r="B41" s="62" t="s">
+      <c r="A41" s="64"/>
+      <c r="B41" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
-      <c r="I41" s="63"/>
-      <c r="J41" s="63"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="68"/>
+      <c r="J41" s="68"/>
     </row>
     <row r="42" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A42" s="59"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="18" t="s">
         <v>33</v>
       </c>
@@ -6436,15 +6487,15 @@
       <c r="F42" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="64" t="s">
+      <c r="G42" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H42" s="64"/>
-      <c r="I42" s="64"/>
-      <c r="J42" s="64"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="69"/>
     </row>
     <row r="43" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A43" s="59"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="13" t="s">
         <v>79</v>
       </c>
@@ -6463,13 +6514,13 @@
         <f>D3</f>
         <v>5000</v>
       </c>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63"/>
     </row>
     <row r="44" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A44" s="59"/>
+      <c r="A44" s="64"/>
       <c r="B44" s="13" t="s">
         <v>81</v>
       </c>
@@ -6488,13 +6539,13 @@
         <f>D4</f>
         <v>0.5</v>
       </c>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
     </row>
     <row r="45" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A45" s="59"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="13" t="s">
         <v>83</v>
       </c>
@@ -6510,15 +6561,15 @@
       <c r="F45" s="4">
         <v>0.2</v>
       </c>
-      <c r="G45" s="58" t="s">
+      <c r="G45" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
     </row>
     <row r="46" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A46" s="59"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="10" t="s">
         <v>86</v>
       </c>
@@ -6537,13 +6588,13 @@
         <f>F43*F44*F45</f>
         <v>500</v>
       </c>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
+      <c r="G46" s="63"/>
+      <c r="H46" s="63"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
     </row>
     <row r="47" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A47" s="59"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="13" t="s">
         <v>88</v>
       </c>
@@ -6559,15 +6610,15 @@
       <c r="F47" s="23">
         <v>0.08</v>
       </c>
-      <c r="G47" s="58" t="s">
+      <c r="G47" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
     </row>
     <row r="48" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A48" s="59"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="10" t="s">
         <v>90</v>
       </c>
@@ -6586,13 +6637,13 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="63"/>
+      <c r="J48" s="63"/>
     </row>
     <row r="49" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A49" s="59"/>
+      <c r="A49" s="64"/>
       <c r="B49" s="13" t="s">
         <v>92</v>
       </c>
@@ -6611,15 +6662,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$H$12,4,FALSE)</f>
         <v>41000</v>
       </c>
-      <c r="G49" s="58" t="s">
+      <c r="G49" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="63"/>
+      <c r="J49" s="63"/>
     </row>
     <row r="50" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A50" s="59"/>
+      <c r="A50" s="64"/>
       <c r="B50" s="16" t="s">
         <v>95</v>
       </c>
@@ -6638,27 +6689,27 @@
         <f>F48*F49</f>
         <v>1640000</v>
       </c>
-      <c r="G50" s="58" t="s">
+      <c r="G50" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="58"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="63"/>
+      <c r="J50" s="63"/>
     </row>
     <row r="51" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A51" s="59"/>
-      <c r="B51" s="66"/>
-      <c r="C51" s="66"/>
-      <c r="D51" s="66"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="66"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="66"/>
-      <c r="I51" s="66"/>
-      <c r="J51" s="67"/>
+      <c r="A51" s="64"/>
+      <c r="B51" s="71"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="71"/>
+      <c r="G51" s="71"/>
+      <c r="H51" s="71"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="72"/>
     </row>
     <row r="52" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A52" s="59"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="13" t="s">
         <v>97</v>
       </c>
@@ -6674,15 +6725,15 @@
       <c r="F52" s="4">
         <v>0.25</v>
       </c>
-      <c r="G52" s="58" t="s">
+      <c r="G52" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
-      <c r="J52" s="58"/>
+      <c r="H52" s="63"/>
+      <c r="I52" s="63"/>
+      <c r="J52" s="63"/>
     </row>
     <row r="53" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A53" s="59"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="13" t="s">
         <v>99</v>
       </c>
@@ -6698,15 +6749,15 @@
       <c r="F53" s="4">
         <v>0.1</v>
       </c>
-      <c r="G53" s="57" t="s">
+      <c r="G53" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="H53" s="57"/>
-      <c r="I53" s="57"/>
-      <c r="J53" s="57"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="62"/>
     </row>
     <row r="54" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A54" s="59"/>
+      <c r="A54" s="64"/>
       <c r="B54" s="16" t="s">
         <v>100</v>
       </c>
@@ -6723,43 +6774,43 @@
         <f>F50*(1-F52)*(1-F53)</f>
         <v>1107000</v>
       </c>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
     </row>
     <row r="56" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="60" t="s">
+      <c r="B56" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="61"/>
-      <c r="D56" s="61"/>
-      <c r="E56" s="61"/>
-      <c r="F56" s="61"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="61"/>
-      <c r="I56" s="61"/>
-      <c r="J56" s="61"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="66"/>
+      <c r="F56" s="66"/>
+      <c r="G56" s="66"/>
+      <c r="H56" s="66"/>
+      <c r="I56" s="66"/>
+      <c r="J56" s="66"/>
     </row>
     <row r="57" spans="1:10" ht="49.35" customHeight="1">
-      <c r="A57" s="59"/>
-      <c r="B57" s="62" t="s">
+      <c r="A57" s="64"/>
+      <c r="B57" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="63"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="63"/>
-      <c r="F57" s="63"/>
-      <c r="G57" s="63"/>
-      <c r="H57" s="63"/>
-      <c r="I57" s="63"/>
-      <c r="J57" s="63"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="68"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="68"/>
+      <c r="J57" s="68"/>
     </row>
     <row r="58" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A58" s="59"/>
+      <c r="A58" s="64"/>
       <c r="B58" s="18" t="s">
         <v>33</v>
       </c>
@@ -6775,15 +6826,15 @@
       <c r="F58" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G58" s="64" t="s">
+      <c r="G58" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H58" s="64"/>
-      <c r="I58" s="64"/>
-      <c r="J58" s="64"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="69"/>
+      <c r="J58" s="69"/>
     </row>
     <row r="59" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A59" s="59"/>
+      <c r="A59" s="64"/>
       <c r="B59" s="13" t="s">
         <v>103</v>
       </c>
@@ -6801,15 +6852,15 @@
         <f>D59</f>
         <v>3.2</v>
       </c>
-      <c r="G59" s="58" t="s">
+      <c r="G59" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
-      <c r="J59" s="58"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="63"/>
+      <c r="J59" s="63"/>
     </row>
     <row r="60" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A60" s="59"/>
+      <c r="A60" s="64"/>
       <c r="B60" s="13" t="s">
         <v>106</v>
       </c>
@@ -6828,13 +6879,13 @@
         <f>E60</f>
         <v>5000</v>
       </c>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="58"/>
-      <c r="J60" s="58"/>
+      <c r="G60" s="63"/>
+      <c r="H60" s="63"/>
+      <c r="I60" s="63"/>
+      <c r="J60" s="63"/>
     </row>
     <row r="61" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A61" s="59"/>
+      <c r="A61" s="64"/>
       <c r="B61" s="13" t="s">
         <v>107</v>
       </c>
@@ -6853,13 +6904,13 @@
         <f>E61</f>
         <v>0.5</v>
       </c>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
-      <c r="J61" s="58"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="63"/>
+      <c r="I61" s="63"/>
+      <c r="J61" s="63"/>
     </row>
     <row r="62" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A62" s="59"/>
+      <c r="A62" s="64"/>
       <c r="B62" s="13" t="s">
         <v>108</v>
       </c>
@@ -6875,15 +6926,15 @@
       <c r="F62" s="5">
         <v>53</v>
       </c>
-      <c r="G62" s="65" t="s">
+      <c r="G62" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="H62" s="65"/>
-      <c r="I62" s="65"/>
-      <c r="J62" s="65"/>
+      <c r="H62" s="70"/>
+      <c r="I62" s="70"/>
+      <c r="J62" s="70"/>
     </row>
     <row r="63" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A63" s="59"/>
+      <c r="A63" s="64"/>
       <c r="B63" s="10" t="s">
         <v>111</v>
       </c>
@@ -6902,13 +6953,13 @@
         <f>F59*F60*F61*F62</f>
         <v>424000</v>
       </c>
-      <c r="G63" s="58"/>
-      <c r="H63" s="58"/>
-      <c r="I63" s="58"/>
-      <c r="J63" s="58"/>
+      <c r="G63" s="63"/>
+      <c r="H63" s="63"/>
+      <c r="I63" s="63"/>
+      <c r="J63" s="63"/>
     </row>
     <row r="64" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A64" s="59"/>
+      <c r="A64" s="64"/>
       <c r="B64" s="13" t="s">
         <v>113</v>
       </c>
@@ -6924,15 +6975,15 @@
       <c r="F64" s="4">
         <v>0.75</v>
       </c>
-      <c r="G64" s="58" t="s">
+      <c r="G64" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="H64" s="58"/>
-      <c r="I64" s="58"/>
-      <c r="J64" s="58"/>
+      <c r="H64" s="63"/>
+      <c r="I64" s="63"/>
+      <c r="J64" s="63"/>
     </row>
     <row r="65" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A65" s="59"/>
+      <c r="A65" s="64"/>
       <c r="B65" s="16" t="s">
         <v>115</v>
       </c>
@@ -6951,25 +7002,25 @@
         <f t="shared" si="4"/>
         <v>318000</v>
       </c>
-      <c r="G65" s="53"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="54"/>
-      <c r="J65" s="55"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="59"/>
+      <c r="J65" s="60"/>
     </row>
     <row r="66" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A66" s="59"/>
-      <c r="B66" s="56"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="56"/>
-      <c r="I66" s="56"/>
-      <c r="J66" s="56"/>
+      <c r="A66" s="64"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="61"/>
+      <c r="G66" s="61"/>
+      <c r="H66" s="61"/>
+      <c r="I66" s="61"/>
+      <c r="J66" s="61"/>
     </row>
     <row r="67" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A67" s="59"/>
+      <c r="A67" s="64"/>
       <c r="B67" s="13" t="s">
         <v>117</v>
       </c>
@@ -6985,15 +7036,15 @@
       <c r="F67" s="4">
         <v>0.25</v>
       </c>
-      <c r="G67" s="57" t="s">
+      <c r="G67" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="H67" s="57"/>
-      <c r="I67" s="57"/>
-      <c r="J67" s="57"/>
+      <c r="H67" s="62"/>
+      <c r="I67" s="62"/>
+      <c r="J67" s="62"/>
     </row>
     <row r="68" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A68" s="59"/>
+      <c r="A68" s="64"/>
       <c r="B68" s="16" t="s">
         <v>118</v>
       </c>
@@ -7010,43 +7061,43 @@
         <f>F65*(1-F67)</f>
         <v>238500</v>
       </c>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="58"/>
-      <c r="J68" s="58"/>
+      <c r="G68" s="63"/>
+      <c r="H68" s="63"/>
+      <c r="I68" s="63"/>
+      <c r="J68" s="63"/>
     </row>
     <row r="70" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A70" s="59" t="s">
+      <c r="A70" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="B70" s="60" t="s">
+      <c r="B70" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C70" s="61"/>
-      <c r="D70" s="61"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="61"/>
-      <c r="G70" s="61"/>
-      <c r="H70" s="61"/>
-      <c r="I70" s="61"/>
-      <c r="J70" s="61"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
+      <c r="H70" s="66"/>
+      <c r="I70" s="66"/>
+      <c r="J70" s="66"/>
     </row>
     <row r="71" spans="1:10" ht="41.45" customHeight="1">
-      <c r="A71" s="59"/>
-      <c r="B71" s="62" t="s">
+      <c r="A71" s="64"/>
+      <c r="B71" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="63"/>
-      <c r="D71" s="63"/>
-      <c r="E71" s="63"/>
-      <c r="F71" s="63"/>
-      <c r="G71" s="63"/>
-      <c r="H71" s="63"/>
-      <c r="I71" s="63"/>
-      <c r="J71" s="63"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="68"/>
+      <c r="F71" s="68"/>
+      <c r="G71" s="68"/>
+      <c r="H71" s="68"/>
+      <c r="I71" s="68"/>
+      <c r="J71" s="68"/>
     </row>
     <row r="72" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A72" s="59"/>
+      <c r="A72" s="64"/>
       <c r="B72" s="18" t="s">
         <v>33</v>
       </c>
@@ -7062,15 +7113,15 @@
       <c r="F72" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G72" s="64" t="s">
+      <c r="G72" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H72" s="64"/>
-      <c r="I72" s="64"/>
-      <c r="J72" s="64"/>
+      <c r="H72" s="69"/>
+      <c r="I72" s="69"/>
+      <c r="J72" s="69"/>
     </row>
     <row r="73" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A73" s="59"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="13" t="s">
         <v>121</v>
       </c>
@@ -7089,15 +7140,15 @@
         <f>E73</f>
         <v>175000</v>
       </c>
-      <c r="G73" s="65" t="s">
+      <c r="G73" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="H73" s="65"/>
-      <c r="I73" s="65"/>
-      <c r="J73" s="65"/>
+      <c r="H73" s="70"/>
+      <c r="I73" s="70"/>
+      <c r="J73" s="70"/>
     </row>
     <row r="74" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A74" s="59"/>
+      <c r="A74" s="64"/>
       <c r="B74" s="13" t="s">
         <v>124</v>
       </c>
@@ -7113,15 +7164,15 @@
       <c r="F74" s="28">
         <v>0.3</v>
       </c>
-      <c r="G74" s="58" t="s">
+      <c r="G74" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="H74" s="58"/>
-      <c r="I74" s="58"/>
-      <c r="J74" s="58"/>
+      <c r="H74" s="63"/>
+      <c r="I74" s="63"/>
+      <c r="J74" s="63"/>
     </row>
     <row r="75" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A75" s="59"/>
+      <c r="A75" s="64"/>
       <c r="B75" s="13" t="s">
         <v>127</v>
       </c>
@@ -7140,15 +7191,15 @@
         <f>IF($D$5="Yes",$G$4*36000,0)</f>
         <v>72000</v>
       </c>
-      <c r="G75" s="58" t="s">
+      <c r="G75" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="H75" s="58"/>
-      <c r="I75" s="58"/>
-      <c r="J75" s="58"/>
+      <c r="H75" s="63"/>
+      <c r="I75" s="63"/>
+      <c r="J75" s="63"/>
     </row>
     <row r="76" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A76" s="59"/>
+      <c r="A76" s="64"/>
       <c r="B76" s="13" t="s">
         <v>130</v>
       </c>
@@ -7167,13 +7218,13 @@
         <f>(F73*F74)+F75</f>
         <v>124500</v>
       </c>
-      <c r="G76" s="58"/>
-      <c r="H76" s="58"/>
-      <c r="I76" s="58"/>
-      <c r="J76" s="58"/>
+      <c r="G76" s="63"/>
+      <c r="H76" s="63"/>
+      <c r="I76" s="63"/>
+      <c r="J76" s="63"/>
     </row>
     <row r="77" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A77" s="59"/>
+      <c r="A77" s="64"/>
       <c r="B77" s="13" t="s">
         <v>132</v>
       </c>
@@ -7189,13 +7240,13 @@
       <c r="F77" s="28">
         <v>0.1</v>
       </c>
-      <c r="G77" s="65"/>
-      <c r="H77" s="65"/>
-      <c r="I77" s="65"/>
-      <c r="J77" s="65"/>
+      <c r="G77" s="70"/>
+      <c r="H77" s="70"/>
+      <c r="I77" s="70"/>
+      <c r="J77" s="70"/>
     </row>
     <row r="78" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A78" s="59"/>
+      <c r="A78" s="64"/>
       <c r="B78" s="16" t="s">
         <v>130</v>
       </c>
@@ -7212,43 +7263,43 @@
         <f>F76*(1-F77)</f>
         <v>112050</v>
       </c>
-      <c r="G78" s="53"/>
-      <c r="H78" s="54"/>
-      <c r="I78" s="54"/>
-      <c r="J78" s="55"/>
+      <c r="G78" s="58"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="59"/>
+      <c r="J78" s="60"/>
     </row>
     <row r="80" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A80" s="59" t="s">
+      <c r="A80" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="B80" s="60" t="s">
+      <c r="B80" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="C80" s="61"/>
-      <c r="D80" s="61"/>
-      <c r="E80" s="61"/>
-      <c r="F80" s="61"/>
-      <c r="G80" s="61"/>
-      <c r="H80" s="61"/>
-      <c r="I80" s="61"/>
-      <c r="J80" s="61"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="66"/>
+      <c r="E80" s="66"/>
+      <c r="F80" s="66"/>
+      <c r="G80" s="66"/>
+      <c r="H80" s="66"/>
+      <c r="I80" s="66"/>
+      <c r="J80" s="66"/>
     </row>
     <row r="81" spans="1:10" ht="78" customHeight="1">
-      <c r="A81" s="59"/>
-      <c r="B81" s="62" t="s">
+      <c r="A81" s="64"/>
+      <c r="B81" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="C81" s="63"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
-      <c r="F81" s="63"/>
-      <c r="G81" s="63"/>
-      <c r="H81" s="63"/>
-      <c r="I81" s="63"/>
-      <c r="J81" s="63"/>
+      <c r="C81" s="68"/>
+      <c r="D81" s="68"/>
+      <c r="E81" s="68"/>
+      <c r="F81" s="68"/>
+      <c r="G81" s="68"/>
+      <c r="H81" s="68"/>
+      <c r="I81" s="68"/>
+      <c r="J81" s="68"/>
     </row>
     <row r="82" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A82" s="59"/>
+      <c r="A82" s="64"/>
       <c r="B82" s="18" t="s">
         <v>33</v>
       </c>
@@ -7264,15 +7315,15 @@
       <c r="F82" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G82" s="64" t="s">
+      <c r="G82" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="H82" s="64"/>
-      <c r="I82" s="64"/>
-      <c r="J82" s="64"/>
+      <c r="H82" s="69"/>
+      <c r="I82" s="69"/>
+      <c r="J82" s="69"/>
     </row>
     <row r="83" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A83" s="59"/>
+      <c r="A83" s="64"/>
       <c r="B83" s="13" t="s">
         <v>137</v>
       </c>
@@ -7291,15 +7342,15 @@
         <f>ROUNDUP(D3/2000,0)</f>
         <v>3</v>
       </c>
-      <c r="G83" s="65" t="s">
+      <c r="G83" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="H83" s="65"/>
-      <c r="I83" s="65"/>
-      <c r="J83" s="65"/>
+      <c r="H83" s="70"/>
+      <c r="I83" s="70"/>
+      <c r="J83" s="70"/>
     </row>
     <row r="84" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A84" s="59"/>
+      <c r="A84" s="64"/>
       <c r="B84" s="13" t="s">
         <v>140</v>
       </c>
@@ -7315,15 +7366,15 @@
       <c r="F84" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G84" s="53" t="s">
+      <c r="G84" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="H84" s="54"/>
-      <c r="I84" s="54"/>
-      <c r="J84" s="55"/>
+      <c r="H84" s="59"/>
+      <c r="I84" s="59"/>
+      <c r="J84" s="60"/>
     </row>
     <row r="85" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A85" s="59"/>
+      <c r="A85" s="64"/>
       <c r="B85" s="13" t="s">
         <v>143</v>
       </c>
@@ -7339,15 +7390,15 @@
       <c r="F85" s="23">
         <v>0.05</v>
       </c>
-      <c r="G85" s="53" t="s">
+      <c r="G85" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="H85" s="54"/>
-      <c r="I85" s="54"/>
-      <c r="J85" s="55"/>
+      <c r="H85" s="59"/>
+      <c r="I85" s="59"/>
+      <c r="J85" s="60"/>
     </row>
     <row r="86" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A86" s="59"/>
+      <c r="A86" s="64"/>
       <c r="B86" s="13" t="s">
         <v>146</v>
       </c>
@@ -7366,15 +7417,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$F$12,2,FALSE)</f>
         <v>50280</v>
       </c>
-      <c r="G86" s="58" t="s">
+      <c r="G86" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="H86" s="58"/>
-      <c r="I86" s="58"/>
-      <c r="J86" s="58"/>
+      <c r="H86" s="63"/>
+      <c r="I86" s="63"/>
+      <c r="J86" s="63"/>
     </row>
     <row r="87" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A87" s="59"/>
+      <c r="A87" s="64"/>
       <c r="B87" s="10" t="s">
         <v>148</v>
       </c>
@@ -7393,13 +7444,13 @@
         <f>F83*(F84+F85)*F86</f>
         <v>18100.800000000003</v>
       </c>
-      <c r="G87" s="58"/>
-      <c r="H87" s="58"/>
-      <c r="I87" s="58"/>
-      <c r="J87" s="58"/>
+      <c r="G87" s="63"/>
+      <c r="H87" s="63"/>
+      <c r="I87" s="63"/>
+      <c r="J87" s="63"/>
     </row>
     <row r="88" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A88" s="59"/>
+      <c r="A88" s="64"/>
       <c r="B88" s="13" t="s">
         <v>150</v>
       </c>
@@ -7415,15 +7466,15 @@
       <c r="F88" s="4">
         <v>0.02</v>
       </c>
-      <c r="G88" s="53" t="s">
+      <c r="G88" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="H88" s="54"/>
-      <c r="I88" s="54"/>
-      <c r="J88" s="55"/>
+      <c r="H88" s="59"/>
+      <c r="I88" s="59"/>
+      <c r="J88" s="60"/>
     </row>
     <row r="89" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A89" s="59"/>
+      <c r="A89" s="64"/>
       <c r="B89" s="10" t="s">
         <v>152</v>
       </c>
@@ -7442,13 +7493,13 @@
         <f>F83*(F86)*F88</f>
         <v>3016.8</v>
       </c>
-      <c r="G89" s="58"/>
-      <c r="H89" s="58"/>
-      <c r="I89" s="58"/>
-      <c r="J89" s="58"/>
+      <c r="G89" s="63"/>
+      <c r="H89" s="63"/>
+      <c r="I89" s="63"/>
+      <c r="J89" s="63"/>
     </row>
     <row r="90" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A90" s="59"/>
+      <c r="A90" s="64"/>
       <c r="B90" s="13" t="s">
         <v>154</v>
       </c>
@@ -7467,15 +7518,15 @@
         <f>$J$4*$D$3</f>
         <v>325000</v>
       </c>
-      <c r="G90" s="58" t="s">
+      <c r="G90" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="H90" s="58"/>
-      <c r="I90" s="58"/>
-      <c r="J90" s="58"/>
+      <c r="H90" s="63"/>
+      <c r="I90" s="63"/>
+      <c r="J90" s="63"/>
     </row>
     <row r="91" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A91" s="59"/>
+      <c r="A91" s="64"/>
       <c r="B91" s="13" t="s">
         <v>157</v>
       </c>
@@ -7494,15 +7545,15 @@
         <f t="shared" si="5"/>
         <v>1200</v>
       </c>
-      <c r="G91" s="53" t="s">
+      <c r="G91" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="H91" s="54"/>
-      <c r="I91" s="54"/>
-      <c r="J91" s="55"/>
+      <c r="H91" s="59"/>
+      <c r="I91" s="59"/>
+      <c r="J91" s="60"/>
     </row>
     <row r="92" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A92" s="59"/>
+      <c r="A92" s="64"/>
       <c r="B92" s="13" t="s">
         <v>160</v>
       </c>
@@ -7521,15 +7572,15 @@
         <f>IF($D$5="Yes",$G$4*4500,0)</f>
         <v>9000</v>
       </c>
-      <c r="G92" s="53" t="s">
+      <c r="G92" s="58" t="s">
         <v>162</v>
       </c>
-      <c r="H92" s="54"/>
-      <c r="I92" s="54"/>
-      <c r="J92" s="55"/>
+      <c r="H92" s="59"/>
+      <c r="I92" s="59"/>
+      <c r="J92" s="60"/>
     </row>
     <row r="93" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A93" s="59"/>
+      <c r="A93" s="64"/>
       <c r="B93" s="29" t="s">
         <v>163</v>
       </c>
@@ -7548,25 +7599,25 @@
         <f>SUM(F87,F89:F92)</f>
         <v>356317.6</v>
       </c>
-      <c r="G93" s="53"/>
-      <c r="H93" s="54"/>
-      <c r="I93" s="54"/>
-      <c r="J93" s="55"/>
+      <c r="G93" s="58"/>
+      <c r="H93" s="59"/>
+      <c r="I93" s="59"/>
+      <c r="J93" s="60"/>
     </row>
     <row r="94" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A94" s="59"/>
-      <c r="B94" s="56"/>
-      <c r="C94" s="56"/>
-      <c r="D94" s="56"/>
-      <c r="E94" s="56"/>
-      <c r="F94" s="56"/>
-      <c r="G94" s="56"/>
-      <c r="H94" s="56"/>
-      <c r="I94" s="56"/>
-      <c r="J94" s="56"/>
+      <c r="A94" s="64"/>
+      <c r="B94" s="61"/>
+      <c r="C94" s="61"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="61"/>
+      <c r="F94" s="61"/>
+      <c r="G94" s="61"/>
+      <c r="H94" s="61"/>
+      <c r="I94" s="61"/>
+      <c r="J94" s="61"/>
     </row>
     <row r="95" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A95" s="59"/>
+      <c r="A95" s="64"/>
       <c r="B95" s="13" t="s">
         <v>165</v>
       </c>
@@ -7582,13 +7633,13 @@
       <c r="F95" s="4">
         <v>0.05</v>
       </c>
-      <c r="G95" s="57"/>
-      <c r="H95" s="57"/>
-      <c r="I95" s="57"/>
-      <c r="J95" s="57"/>
+      <c r="G95" s="62"/>
+      <c r="H95" s="62"/>
+      <c r="I95" s="62"/>
+      <c r="J95" s="62"/>
     </row>
     <row r="96" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A96" s="59"/>
+      <c r="A96" s="64"/>
       <c r="B96" s="16"/>
       <c r="C96" s="16"/>
       <c r="D96" s="26">
@@ -7603,10 +7654,10 @@
         <f>F93*(1+F95)</f>
         <v>374133.48</v>
       </c>
-      <c r="G96" s="58"/>
-      <c r="H96" s="58"/>
-      <c r="I96" s="58"/>
-      <c r="J96" s="58"/>
+      <c r="G96" s="63"/>
+      <c r="H96" s="63"/>
+      <c r="I96" s="63"/>
+      <c r="J96" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="82">
@@ -7718,6 +7769,502 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9F39E0-A2D0-4352-951C-B83BA4C81993}">
+  <dimension ref="E2:H43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36:H43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="8" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:8">
+      <c r="E2" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="5:8">
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3">
+        <v>1500</v>
+      </c>
+      <c r="G3">
+        <v>1500</v>
+      </c>
+      <c r="H3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8">
+      <c r="E4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="54">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="54">
+        <v>0.6</v>
+      </c>
+      <c r="H4" s="54">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8">
+      <c r="E5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="54">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G5" s="54">
+        <v>0.6</v>
+      </c>
+      <c r="H5" s="54">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8">
+      <c r="E6" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="54">
+        <v>0.15</v>
+      </c>
+      <c r="G6" s="54">
+        <v>0.15</v>
+      </c>
+      <c r="H6" s="54">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8">
+      <c r="E7" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="F7">
+        <v>1800</v>
+      </c>
+      <c r="G7">
+        <v>1800</v>
+      </c>
+      <c r="H7">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8">
+      <c r="E8" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="F8" s="54">
+        <v>0.33</v>
+      </c>
+      <c r="G8" s="54">
+        <v>0.33</v>
+      </c>
+      <c r="H8" s="54">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8">
+      <c r="E9" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="54">
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="54">
+        <v>0.25</v>
+      </c>
+      <c r="H9" s="54">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8">
+      <c r="E10" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="54">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8">
+      <c r="E13" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8">
+      <c r="E14" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="F14" s="54">
+        <v>0.2</v>
+      </c>
+      <c r="G14" s="54">
+        <v>0.2</v>
+      </c>
+      <c r="H14" s="54">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8">
+      <c r="E15" s="53" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" s="54">
+        <v>0.08</v>
+      </c>
+      <c r="G15" s="54">
+        <v>0.08</v>
+      </c>
+      <c r="H15" s="54">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8">
+      <c r="E16" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="54">
+        <v>0.25</v>
+      </c>
+      <c r="G16" s="54">
+        <v>0.25</v>
+      </c>
+      <c r="H16" s="54">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8">
+      <c r="E17" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="54">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8">
+      <c r="E20" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8">
+      <c r="E21" s="57" t="s">
+        <v>176</v>
+      </c>
+      <c r="F21">
+        <v>3.2</v>
+      </c>
+      <c r="G21">
+        <v>3.2</v>
+      </c>
+      <c r="H21">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8">
+      <c r="E22" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="F22">
+        <v>53</v>
+      </c>
+      <c r="G22">
+        <v>53</v>
+      </c>
+      <c r="H22">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8">
+      <c r="E23" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="F23" s="54">
+        <v>0.75</v>
+      </c>
+      <c r="G23" s="54">
+        <v>0.75</v>
+      </c>
+      <c r="H23" s="54">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8">
+      <c r="E24" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="54">
+        <v>0.25</v>
+      </c>
+      <c r="G24" s="54">
+        <v>0.25</v>
+      </c>
+      <c r="H24" s="54">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8">
+      <c r="E27" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8">
+      <c r="E28" s="57" t="s">
+        <v>180</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <v>20</v>
+      </c>
+      <c r="H28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8">
+      <c r="E29" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="F29">
+        <v>5000</v>
+      </c>
+      <c r="G29">
+        <v>5000</v>
+      </c>
+      <c r="H29">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="30" spans="5:8">
+      <c r="E30" t="s">
+        <v>182</v>
+      </c>
+      <c r="F30">
+        <v>50000</v>
+      </c>
+      <c r="G30">
+        <v>50000</v>
+      </c>
+      <c r="H30">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8">
+      <c r="E31" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="F31" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G31" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="H31" s="54">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="32" spans="5:8">
+      <c r="E32" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32">
+        <v>36000</v>
+      </c>
+      <c r="G32">
+        <v>36000</v>
+      </c>
+      <c r="H32">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8">
+      <c r="E33" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="G33" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H33" s="54">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8">
+      <c r="E36" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8">
+      <c r="E37" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37">
+        <v>2000</v>
+      </c>
+      <c r="G37">
+        <v>2000</v>
+      </c>
+      <c r="H37">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="38" spans="5:8">
+      <c r="E38" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="54">
+        <v>0.15</v>
+      </c>
+      <c r="G38" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H38" s="54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="5:8">
+      <c r="E39" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="F39" s="54">
+        <v>0.5</v>
+      </c>
+      <c r="G39" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="H39" s="54">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="40" spans="5:8">
+      <c r="E40" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="F40" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="G40" s="54">
+        <v>0.05</v>
+      </c>
+      <c r="H40" s="54">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="41" spans="5:8">
+      <c r="E41" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="F41">
+        <v>1200</v>
+      </c>
+      <c r="G41">
+        <v>1200</v>
+      </c>
+      <c r="H41">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="42" spans="5:8">
+      <c r="E42" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="F42">
+        <v>4500</v>
+      </c>
+      <c r="G42">
+        <v>4500</v>
+      </c>
+      <c r="H42">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="43" spans="5:8">
+      <c r="E43" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="54">
+        <v>0.05</v>
+      </c>
+      <c r="G43" s="54">
+        <v>0.05</v>
+      </c>
+      <c r="H43" s="54">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB613458-C399-4236-80B2-A648D5D4F436}">
   <dimension ref="E2:K12"/>
   <sheetViews>
@@ -7737,19 +8284,19 @@
   <sheetData>
     <row r="2" spans="5:11">
       <c r="E2" s="3" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="5:11">
@@ -7772,7 +8319,7 @@
     </row>
     <row r="4" spans="5:11">
       <c r="E4" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="F4">
         <v>26740</v>
@@ -7789,7 +8336,7 @@
     </row>
     <row r="5" spans="5:11">
       <c r="E5" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="F5">
         <v>9300</v>
@@ -7807,7 +8354,7 @@
     </row>
     <row r="6" spans="5:11">
       <c r="E6" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="F6">
         <v>48492</v>
@@ -7824,7 +8371,7 @@
     </row>
     <row r="7" spans="5:11">
       <c r="E7" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="F7">
         <v>21000</v>
@@ -7841,7 +8388,7 @@
     </row>
     <row r="8" spans="5:11">
       <c r="E8" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="F8">
         <v>17400</v>
@@ -7858,7 +8405,7 @@
     </row>
     <row r="9" spans="5:11">
       <c r="E9" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="F9">
         <v>13320</v>
@@ -7875,7 +8422,7 @@
     </row>
     <row r="10" spans="5:11">
       <c r="E10" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="F10" s="8">
         <v>44234</v>
@@ -7892,7 +8439,7 @@
     </row>
     <row r="11" spans="5:11">
       <c r="E11" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="F11" s="8">
         <v>34786</v>
@@ -7909,7 +8456,7 @@
     </row>
     <row r="12" spans="5:11">
       <c r="E12" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="F12">
         <v>59000</v>
@@ -7922,235 +8469,6 @@
       </c>
       <c r="I12">
         <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9F39E0-A2D0-4352-951C-B83BA4C81993}">
-  <dimension ref="E2:H19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="5" max="5" width="42.5703125" customWidth="1"/>
-    <col min="6" max="8" width="10" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="5:8">
-      <c r="E2" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="5:8">
-      <c r="E3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3">
-        <v>1500</v>
-      </c>
-      <c r="G3">
-        <v>1500</v>
-      </c>
-      <c r="H3">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="4" spans="5:8">
-      <c r="E4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F4" s="69">
-        <v>0.6</v>
-      </c>
-      <c r="G4" s="69">
-        <v>0.6</v>
-      </c>
-      <c r="H4" s="69">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="5:8">
-      <c r="E5" t="s">
-        <v>183</v>
-      </c>
-      <c r="F5" s="69">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G5" s="69">
-        <v>0.6</v>
-      </c>
-      <c r="H5" s="69">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="6" spans="5:8">
-      <c r="E6" s="68" t="s">
-        <v>184</v>
-      </c>
-      <c r="F6" s="69">
-        <v>0.15</v>
-      </c>
-      <c r="G6" s="69">
-        <v>0.15</v>
-      </c>
-      <c r="H6" s="69">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="7" spans="5:8">
-      <c r="E7" s="68" t="s">
-        <v>183</v>
-      </c>
-      <c r="F7" s="69">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G7" s="69">
-        <v>0.6</v>
-      </c>
-      <c r="H7" s="69">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="8" spans="5:8">
-      <c r="E8" s="68" t="s">
-        <v>185</v>
-      </c>
-      <c r="F8">
-        <v>1800</v>
-      </c>
-      <c r="G8">
-        <v>1800</v>
-      </c>
-      <c r="H8">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="9" spans="5:8">
-      <c r="E9" s="68" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" s="69">
-        <v>0.33</v>
-      </c>
-      <c r="G9" s="69">
-        <v>0.33</v>
-      </c>
-      <c r="H9" s="69">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="10" spans="5:8">
-      <c r="E10" s="68" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="69">
-        <v>0.25</v>
-      </c>
-      <c r="G10" s="69">
-        <v>0.25</v>
-      </c>
-      <c r="H10" s="69">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="11" spans="5:8">
-      <c r="E11" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="69">
-        <v>0.1</v>
-      </c>
-      <c r="G11" s="69">
-        <v>0.1</v>
-      </c>
-      <c r="H11" s="69">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="15" spans="5:8">
-      <c r="E15" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="5:8">
-      <c r="E16" s="68" t="s">
-        <v>187</v>
-      </c>
-      <c r="F16" s="69">
-        <v>0.2</v>
-      </c>
-      <c r="G16" s="69">
-        <v>0.2</v>
-      </c>
-      <c r="H16" s="69">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8">
-      <c r="E17" s="68" t="s">
-        <v>188</v>
-      </c>
-      <c r="F17" s="69">
-        <v>0.08</v>
-      </c>
-      <c r="G17" s="69">
-        <v>0.08</v>
-      </c>
-      <c r="H17" s="69">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="18" spans="5:8">
-      <c r="E18" s="68" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="69">
-        <v>0.25</v>
-      </c>
-      <c r="G18" s="69">
-        <v>0.25</v>
-      </c>
-      <c r="H18" s="69">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8">
-      <c r="E19" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="69">
-        <v>0.1</v>
-      </c>
-      <c r="G19" s="69">
-        <v>0.1</v>
-      </c>
-      <c r="H19" s="69">
-        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -8173,50 +8491,50 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
captcha added & UI updated
</commit_message>
<xml_diff>
--- a/public/formula.xlsx
+++ b/public/formula.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28605"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28627"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sangforltd-my.sharepoint.com/personal/akarsh_jain_sangfor_com/Documents/Sangfor Access Secure Collaterals/Sales and Ordering Guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{187293EE-8507-4B20-8B27-AB007DC77401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75E07665-2070-413F-BA46-3C4186FCA02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-700" yWindow="-20700" windowWidth="29600" windowHeight="19760" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-700" yWindow="-20700" windowWidth="29600" windowHeight="19760" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SASE ROI - Original" sheetId="1" r:id="rId1"/>
@@ -626,7 +626,7 @@
     <t>Indonesia</t>
   </si>
   <si>
-    <t>Hongkong</t>
+    <t>Hong Kong</t>
   </si>
   <si>
     <t>Thailand</t>
@@ -644,7 +644,7 @@
     <t>Turkey</t>
   </si>
   <si>
-    <t>UAE</t>
+    <t>United Arab Emirates</t>
   </si>
   <si>
     <t>Original Calculator File</t>
@@ -1108,32 +1108,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1145,12 +1121,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3710,37 +3710,37 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="13.7" customHeight="1">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
     </row>
     <row r="17" spans="1:10" ht="45.6" customHeight="1">
-      <c r="A17" s="64"/>
-      <c r="B17" s="67" t="s">
+      <c r="A17" s="58"/>
+      <c r="B17" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
     </row>
     <row r="18" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A18" s="64"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="18" t="s">
         <v>33</v>
       </c>
@@ -3756,15 +3756,15 @@
       <c r="F18" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="69" t="s">
+      <c r="G18" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
     </row>
     <row r="19" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A19" s="64"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="13" t="s">
         <v>36</v>
       </c>
@@ -3783,15 +3783,15 @@
         <f>D19</f>
         <v>4</v>
       </c>
-      <c r="G19" s="63" t="s">
+      <c r="G19" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
     </row>
     <row r="20" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A20" s="64"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="13" t="s">
         <v>39</v>
       </c>
@@ -3807,15 +3807,15 @@
       <c r="F20" s="23">
         <v>0.6</v>
       </c>
-      <c r="G20" s="63" t="s">
+      <c r="G20" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
     </row>
     <row r="21" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A21" s="64"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="13" t="s">
         <v>42</v>
       </c>
@@ -3831,15 +3831,15 @@
       <c r="F21" s="23">
         <v>0.65</v>
       </c>
-      <c r="G21" s="63" t="s">
+      <c r="G21" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="63"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="64"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="19" t="s">
         <v>45</v>
       </c>
@@ -3858,13 +3858,13 @@
         <f>ROUNDUP(F19*F20*F21,0)</f>
         <v>2</v>
       </c>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="64"/>
+      <c r="A23" s="58"/>
       <c r="B23" s="13" t="s">
         <v>47</v>
       </c>
@@ -3880,15 +3880,15 @@
       <c r="F23" s="23">
         <v>0.15</v>
       </c>
-      <c r="G23" s="63" t="s">
+      <c r="G23" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
     </row>
     <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="64"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="13" t="s">
         <v>49</v>
       </c>
@@ -3904,15 +3904,15 @@
       <c r="F24" s="23">
         <v>0.65</v>
       </c>
-      <c r="G24" s="63" t="s">
+      <c r="G24" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
     </row>
     <row r="25" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A25" s="64"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="19" t="s">
         <v>50</v>
       </c>
@@ -3931,13 +3931,13 @@
         <f>ROUNDUP(F19*F23*F24,0)</f>
         <v>1</v>
       </c>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
     </row>
     <row r="26" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A26" s="64"/>
+      <c r="A26" s="58"/>
       <c r="B26" s="13" t="s">
         <v>52</v>
       </c>
@@ -3956,15 +3956,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$F$12,2,FALSE)</f>
         <v>50280</v>
       </c>
-      <c r="G26" s="63" t="s">
+      <c r="G26" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="63"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="63"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
     </row>
     <row r="27" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A27" s="64"/>
+      <c r="A27" s="58"/>
       <c r="B27" s="20" t="s">
         <v>55</v>
       </c>
@@ -3983,27 +3983,27 @@
         <f>(F22+F25)*F26</f>
         <v>150840</v>
       </c>
-      <c r="G27" s="63" t="s">
+      <c r="G27" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
     </row>
     <row r="28" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A28" s="64"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="72"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="66"/>
+      <c r="J28" s="67"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="64"/>
+      <c r="A29" s="58"/>
       <c r="B29" s="13" t="s">
         <v>58</v>
       </c>
@@ -4022,15 +4022,15 @@
         <f>D29</f>
         <v>3</v>
       </c>
-      <c r="G29" s="63" t="s">
+      <c r="G29" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="63"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="63"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="64"/>
+      <c r="A30" s="58"/>
       <c r="B30" s="13" t="s">
         <v>61</v>
       </c>
@@ -4046,15 +4046,15 @@
       <c r="F30" s="23">
         <v>0.33</v>
       </c>
-      <c r="G30" s="63" t="s">
+      <c r="G30" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="63"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="63"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
     </row>
     <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="64"/>
+      <c r="A31" s="58"/>
       <c r="B31" s="13" t="s">
         <v>63</v>
       </c>
@@ -4070,15 +4070,15 @@
       <c r="F31" s="23">
         <v>0.65</v>
       </c>
-      <c r="G31" s="63" t="s">
+      <c r="G31" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
     </row>
     <row r="32" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A32" s="64"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
@@ -4097,13 +4097,13 @@
         <f>ROUNDUP(F29*F30*F31,0)</f>
         <v>1</v>
       </c>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
     </row>
     <row r="33" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A33" s="64"/>
+      <c r="A33" s="58"/>
       <c r="B33" s="13" t="s">
         <v>66</v>
       </c>
@@ -4122,15 +4122,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$G$12,3,FALSE)</f>
         <v>46862</v>
       </c>
-      <c r="G33" s="63" t="s">
+      <c r="G33" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
     </row>
     <row r="34" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A34" s="64"/>
+      <c r="A34" s="58"/>
       <c r="B34" s="16" t="s">
         <v>68</v>
       </c>
@@ -4149,27 +4149,27 @@
         <f>F33*F32</f>
         <v>46862</v>
       </c>
-      <c r="G34" s="63" t="s">
+      <c r="G34" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="63"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="62"/>
     </row>
     <row r="35" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A35" s="64"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="61"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
     </row>
     <row r="36" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A36" s="64"/>
+      <c r="A36" s="58"/>
       <c r="B36" s="13" t="s">
         <v>70</v>
       </c>
@@ -4185,15 +4185,15 @@
       <c r="F36" s="4">
         <v>0.25</v>
       </c>
-      <c r="G36" s="63" t="s">
+      <c r="G36" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="H36" s="63"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="63"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
     </row>
     <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="64"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="13" t="s">
         <v>73</v>
       </c>
@@ -4209,15 +4209,15 @@
       <c r="F37" s="4">
         <v>0.1</v>
       </c>
-      <c r="G37" s="62" t="s">
+      <c r="G37" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="H37" s="62"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="62"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="65"/>
     </row>
     <row r="38" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A38" s="64"/>
+      <c r="A38" s="58"/>
       <c r="B38" s="16" t="s">
         <v>76</v>
       </c>
@@ -4234,43 +4234,43 @@
         <f>(F27+F34)*(1-F36)*(1-F37)</f>
         <v>133448.85</v>
       </c>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
     </row>
     <row r="40" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="65" t="s">
+      <c r="B40" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="66"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="66"/>
-      <c r="I40" s="66"/>
-      <c r="J40" s="66"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="64"/>
+      <c r="J40" s="64"/>
     </row>
     <row r="41" spans="1:10" ht="45" customHeight="1">
-      <c r="A41" s="64"/>
-      <c r="B41" s="67" t="s">
+      <c r="A41" s="58"/>
+      <c r="B41" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="68"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
     </row>
     <row r="42" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A42" s="64"/>
+      <c r="A42" s="58"/>
       <c r="B42" s="18" t="s">
         <v>33</v>
       </c>
@@ -4286,15 +4286,15 @@
       <c r="F42" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="69" t="s">
+      <c r="G42" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H42" s="69"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="69"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="61"/>
     </row>
     <row r="43" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A43" s="64"/>
+      <c r="A43" s="58"/>
       <c r="B43" s="13" t="s">
         <v>79</v>
       </c>
@@ -4313,13 +4313,13 @@
         <f>D3</f>
         <v>5000</v>
       </c>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
     </row>
     <row r="44" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A44" s="64"/>
+      <c r="A44" s="58"/>
       <c r="B44" s="13" t="s">
         <v>81</v>
       </c>
@@ -4338,13 +4338,13 @@
         <f>D4</f>
         <v>0.5</v>
       </c>
-      <c r="G44" s="63"/>
-      <c r="H44" s="63"/>
-      <c r="I44" s="63"/>
-      <c r="J44" s="63"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
     </row>
     <row r="45" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A45" s="64"/>
+      <c r="A45" s="58"/>
       <c r="B45" s="13" t="s">
         <v>83</v>
       </c>
@@ -4360,15 +4360,15 @@
       <c r="F45" s="4">
         <v>0.2</v>
       </c>
-      <c r="G45" s="63" t="s">
+      <c r="G45" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
     </row>
     <row r="46" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A46" s="64"/>
+      <c r="A46" s="58"/>
       <c r="B46" s="10" t="s">
         <v>86</v>
       </c>
@@ -4387,13 +4387,13 @@
         <f>F43*F44*F45</f>
         <v>500</v>
       </c>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="63"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="62"/>
+      <c r="J46" s="62"/>
     </row>
     <row r="47" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A47" s="64"/>
+      <c r="A47" s="58"/>
       <c r="B47" s="13" t="s">
         <v>88</v>
       </c>
@@ -4409,15 +4409,15 @@
       <c r="F47" s="23">
         <v>0.08</v>
       </c>
-      <c r="G47" s="63" t="s">
+      <c r="G47" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="62"/>
     </row>
     <row r="48" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A48" s="64"/>
+      <c r="A48" s="58"/>
       <c r="B48" s="10" t="s">
         <v>90</v>
       </c>
@@ -4436,13 +4436,13 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="G48" s="63"/>
-      <c r="H48" s="63"/>
-      <c r="I48" s="63"/>
-      <c r="J48" s="63"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="62"/>
+      <c r="J48" s="62"/>
     </row>
     <row r="49" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A49" s="64"/>
+      <c r="A49" s="58"/>
       <c r="B49" s="13" t="s">
         <v>92</v>
       </c>
@@ -4461,15 +4461,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$H$12,4,FALSE)</f>
         <v>41000</v>
       </c>
-      <c r="G49" s="63" t="s">
+      <c r="G49" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="H49" s="63"/>
-      <c r="I49" s="63"/>
-      <c r="J49" s="63"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="62"/>
     </row>
     <row r="50" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A50" s="64"/>
+      <c r="A50" s="58"/>
       <c r="B50" s="16" t="s">
         <v>95</v>
       </c>
@@ -4488,27 +4488,27 @@
         <f>F48*F49</f>
         <v>1640000</v>
       </c>
-      <c r="G50" s="63" t="s">
+      <c r="G50" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="H50" s="63"/>
-      <c r="I50" s="63"/>
-      <c r="J50" s="63"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
     </row>
     <row r="51" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A51" s="64"/>
-      <c r="B51" s="71"/>
-      <c r="C51" s="71"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="71"/>
-      <c r="F51" s="71"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="71"/>
-      <c r="I51" s="71"/>
-      <c r="J51" s="72"/>
+      <c r="A51" s="58"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="66"/>
+      <c r="F51" s="66"/>
+      <c r="G51" s="66"/>
+      <c r="H51" s="66"/>
+      <c r="I51" s="66"/>
+      <c r="J51" s="67"/>
     </row>
     <row r="52" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A52" s="64"/>
+      <c r="A52" s="58"/>
       <c r="B52" s="13" t="s">
         <v>97</v>
       </c>
@@ -4524,15 +4524,15 @@
       <c r="F52" s="4">
         <v>0.25</v>
       </c>
-      <c r="G52" s="63" t="s">
+      <c r="G52" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="H52" s="63"/>
-      <c r="I52" s="63"/>
-      <c r="J52" s="63"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="62"/>
+      <c r="J52" s="62"/>
     </row>
     <row r="53" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A53" s="64"/>
+      <c r="A53" s="58"/>
       <c r="B53" s="13" t="s">
         <v>99</v>
       </c>
@@ -4548,15 +4548,15 @@
       <c r="F53" s="4">
         <v>0.1</v>
       </c>
-      <c r="G53" s="62" t="s">
+      <c r="G53" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="H53" s="62"/>
-      <c r="I53" s="62"/>
-      <c r="J53" s="62"/>
+      <c r="H53" s="65"/>
+      <c r="I53" s="65"/>
+      <c r="J53" s="65"/>
     </row>
     <row r="54" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A54" s="64"/>
+      <c r="A54" s="58"/>
       <c r="B54" s="16" t="s">
         <v>100</v>
       </c>
@@ -4573,43 +4573,43 @@
         <f>F50*(1-F52)*(1-F53)</f>
         <v>1107000</v>
       </c>
-      <c r="G54" s="63"/>
-      <c r="H54" s="63"/>
-      <c r="I54" s="63"/>
-      <c r="J54" s="63"/>
+      <c r="G54" s="62"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="62"/>
+      <c r="J54" s="62"/>
     </row>
     <row r="56" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A56" s="64" t="s">
+      <c r="A56" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="65" t="s">
+      <c r="B56" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="66"/>
-      <c r="D56" s="66"/>
-      <c r="E56" s="66"/>
-      <c r="F56" s="66"/>
-      <c r="G56" s="66"/>
-      <c r="H56" s="66"/>
-      <c r="I56" s="66"/>
-      <c r="J56" s="66"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="64"/>
+      <c r="F56" s="64"/>
+      <c r="G56" s="64"/>
+      <c r="H56" s="64"/>
+      <c r="I56" s="64"/>
+      <c r="J56" s="64"/>
     </row>
     <row r="57" spans="1:10" ht="49.35" customHeight="1">
-      <c r="A57" s="64"/>
-      <c r="B57" s="67" t="s">
+      <c r="A57" s="58"/>
+      <c r="B57" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="68"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="68"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="68"/>
-      <c r="H57" s="68"/>
-      <c r="I57" s="68"/>
-      <c r="J57" s="68"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="60"/>
+      <c r="I57" s="60"/>
+      <c r="J57" s="60"/>
     </row>
     <row r="58" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A58" s="64"/>
+      <c r="A58" s="58"/>
       <c r="B58" s="18" t="s">
         <v>33</v>
       </c>
@@ -4625,15 +4625,15 @@
       <c r="F58" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G58" s="69" t="s">
+      <c r="G58" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H58" s="69"/>
-      <c r="I58" s="69"/>
-      <c r="J58" s="69"/>
+      <c r="H58" s="61"/>
+      <c r="I58" s="61"/>
+      <c r="J58" s="61"/>
     </row>
     <row r="59" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A59" s="64"/>
+      <c r="A59" s="58"/>
       <c r="B59" s="13" t="s">
         <v>103</v>
       </c>
@@ -4651,15 +4651,15 @@
         <f>D59</f>
         <v>3.2</v>
       </c>
-      <c r="G59" s="63" t="s">
+      <c r="G59" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="H59" s="63"/>
-      <c r="I59" s="63"/>
-      <c r="J59" s="63"/>
+      <c r="H59" s="62"/>
+      <c r="I59" s="62"/>
+      <c r="J59" s="62"/>
     </row>
     <row r="60" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A60" s="64"/>
+      <c r="A60" s="58"/>
       <c r="B60" s="13" t="s">
         <v>106</v>
       </c>
@@ -4678,13 +4678,13 @@
         <f>E60</f>
         <v>5000</v>
       </c>
-      <c r="G60" s="63"/>
-      <c r="H60" s="63"/>
-      <c r="I60" s="63"/>
-      <c r="J60" s="63"/>
+      <c r="G60" s="62"/>
+      <c r="H60" s="62"/>
+      <c r="I60" s="62"/>
+      <c r="J60" s="62"/>
     </row>
     <row r="61" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A61" s="64"/>
+      <c r="A61" s="58"/>
       <c r="B61" s="13" t="s">
         <v>107</v>
       </c>
@@ -4703,13 +4703,13 @@
         <f>E61</f>
         <v>0.5</v>
       </c>
-      <c r="G61" s="63"/>
-      <c r="H61" s="63"/>
-      <c r="I61" s="63"/>
-      <c r="J61" s="63"/>
+      <c r="G61" s="62"/>
+      <c r="H61" s="62"/>
+      <c r="I61" s="62"/>
+      <c r="J61" s="62"/>
     </row>
     <row r="62" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A62" s="64"/>
+      <c r="A62" s="58"/>
       <c r="B62" s="13" t="s">
         <v>108</v>
       </c>
@@ -4725,15 +4725,15 @@
       <c r="F62" s="5">
         <v>53</v>
       </c>
-      <c r="G62" s="70" t="s">
+      <c r="G62" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="H62" s="70"/>
-      <c r="I62" s="70"/>
-      <c r="J62" s="70"/>
+      <c r="H62" s="69"/>
+      <c r="I62" s="69"/>
+      <c r="J62" s="69"/>
     </row>
     <row r="63" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A63" s="64"/>
+      <c r="A63" s="58"/>
       <c r="B63" s="10" t="s">
         <v>111</v>
       </c>
@@ -4752,13 +4752,13 @@
         <f>F59*F60*F61*F62</f>
         <v>424000</v>
       </c>
-      <c r="G63" s="63"/>
-      <c r="H63" s="63"/>
-      <c r="I63" s="63"/>
-      <c r="J63" s="63"/>
+      <c r="G63" s="62"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="62"/>
+      <c r="J63" s="62"/>
     </row>
     <row r="64" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A64" s="64"/>
+      <c r="A64" s="58"/>
       <c r="B64" s="13" t="s">
         <v>113</v>
       </c>
@@ -4774,15 +4774,15 @@
       <c r="F64" s="4">
         <v>0.75</v>
       </c>
-      <c r="G64" s="63" t="s">
+      <c r="G64" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H64" s="63"/>
-      <c r="I64" s="63"/>
-      <c r="J64" s="63"/>
+      <c r="H64" s="62"/>
+      <c r="I64" s="62"/>
+      <c r="J64" s="62"/>
     </row>
     <row r="65" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A65" s="64"/>
+      <c r="A65" s="58"/>
       <c r="B65" s="16" t="s">
         <v>115</v>
       </c>
@@ -4801,25 +4801,25 @@
         <f t="shared" si="4"/>
         <v>318000</v>
       </c>
-      <c r="G65" s="58"/>
-      <c r="H65" s="59"/>
-      <c r="I65" s="59"/>
-      <c r="J65" s="60"/>
+      <c r="G65" s="70"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71"/>
+      <c r="J65" s="72"/>
     </row>
     <row r="66" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A66" s="64"/>
-      <c r="B66" s="61"/>
-      <c r="C66" s="61"/>
-      <c r="D66" s="61"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="61"/>
-      <c r="G66" s="61"/>
-      <c r="H66" s="61"/>
-      <c r="I66" s="61"/>
-      <c r="J66" s="61"/>
+      <c r="A66" s="58"/>
+      <c r="B66" s="68"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="68"/>
+      <c r="H66" s="68"/>
+      <c r="I66" s="68"/>
+      <c r="J66" s="68"/>
     </row>
     <row r="67" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A67" s="64"/>
+      <c r="A67" s="58"/>
       <c r="B67" s="13" t="s">
         <v>117</v>
       </c>
@@ -4835,15 +4835,15 @@
       <c r="F67" s="4">
         <v>0.25</v>
       </c>
-      <c r="G67" s="62" t="s">
+      <c r="G67" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="H67" s="62"/>
-      <c r="I67" s="62"/>
-      <c r="J67" s="62"/>
+      <c r="H67" s="65"/>
+      <c r="I67" s="65"/>
+      <c r="J67" s="65"/>
     </row>
     <row r="68" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A68" s="64"/>
+      <c r="A68" s="58"/>
       <c r="B68" s="16" t="s">
         <v>118</v>
       </c>
@@ -4860,43 +4860,43 @@
         <f>F65*(1-F67)</f>
         <v>238500</v>
       </c>
-      <c r="G68" s="63"/>
-      <c r="H68" s="63"/>
-      <c r="I68" s="63"/>
-      <c r="J68" s="63"/>
+      <c r="G68" s="62"/>
+      <c r="H68" s="62"/>
+      <c r="I68" s="62"/>
+      <c r="J68" s="62"/>
     </row>
     <row r="70" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A70" s="64" t="s">
+      <c r="A70" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="B70" s="65" t="s">
+      <c r="B70" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="C70" s="66"/>
-      <c r="D70" s="66"/>
-      <c r="E70" s="66"/>
-      <c r="F70" s="66"/>
-      <c r="G70" s="66"/>
-      <c r="H70" s="66"/>
-      <c r="I70" s="66"/>
-      <c r="J70" s="66"/>
+      <c r="C70" s="64"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="64"/>
+      <c r="F70" s="64"/>
+      <c r="G70" s="64"/>
+      <c r="H70" s="64"/>
+      <c r="I70" s="64"/>
+      <c r="J70" s="64"/>
     </row>
     <row r="71" spans="1:10" ht="41.45" customHeight="1">
-      <c r="A71" s="64"/>
-      <c r="B71" s="67" t="s">
+      <c r="A71" s="58"/>
+      <c r="B71" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="68"/>
-      <c r="D71" s="68"/>
-      <c r="E71" s="68"/>
-      <c r="F71" s="68"/>
-      <c r="G71" s="68"/>
-      <c r="H71" s="68"/>
-      <c r="I71" s="68"/>
-      <c r="J71" s="68"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="60"/>
+      <c r="F71" s="60"/>
+      <c r="G71" s="60"/>
+      <c r="H71" s="60"/>
+      <c r="I71" s="60"/>
+      <c r="J71" s="60"/>
     </row>
     <row r="72" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A72" s="64"/>
+      <c r="A72" s="58"/>
       <c r="B72" s="18" t="s">
         <v>33</v>
       </c>
@@ -4912,15 +4912,15 @@
       <c r="F72" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G72" s="69" t="s">
+      <c r="G72" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H72" s="69"/>
-      <c r="I72" s="69"/>
-      <c r="J72" s="69"/>
+      <c r="H72" s="61"/>
+      <c r="I72" s="61"/>
+      <c r="J72" s="61"/>
     </row>
     <row r="73" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A73" s="64"/>
+      <c r="A73" s="58"/>
       <c r="B73" s="13" t="s">
         <v>121</v>
       </c>
@@ -4939,15 +4939,15 @@
         <f>E73</f>
         <v>175000</v>
       </c>
-      <c r="G73" s="70" t="s">
+      <c r="G73" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="H73" s="70"/>
-      <c r="I73" s="70"/>
-      <c r="J73" s="70"/>
+      <c r="H73" s="69"/>
+      <c r="I73" s="69"/>
+      <c r="J73" s="69"/>
     </row>
     <row r="74" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A74" s="64"/>
+      <c r="A74" s="58"/>
       <c r="B74" s="13" t="s">
         <v>124</v>
       </c>
@@ -4963,15 +4963,15 @@
       <c r="F74" s="28">
         <v>0.3</v>
       </c>
-      <c r="G74" s="63" t="s">
+      <c r="G74" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="H74" s="63"/>
-      <c r="I74" s="63"/>
-      <c r="J74" s="63"/>
+      <c r="H74" s="62"/>
+      <c r="I74" s="62"/>
+      <c r="J74" s="62"/>
     </row>
     <row r="75" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A75" s="64"/>
+      <c r="A75" s="58"/>
       <c r="B75" s="13" t="s">
         <v>127</v>
       </c>
@@ -4990,15 +4990,15 @@
         <f>IF($D$5="Yes",$G$4*36000,0)</f>
         <v>72000</v>
       </c>
-      <c r="G75" s="63" t="s">
+      <c r="G75" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="H75" s="63"/>
-      <c r="I75" s="63"/>
-      <c r="J75" s="63"/>
+      <c r="H75" s="62"/>
+      <c r="I75" s="62"/>
+      <c r="J75" s="62"/>
     </row>
     <row r="76" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A76" s="64"/>
+      <c r="A76" s="58"/>
       <c r="B76" s="13" t="s">
         <v>130</v>
       </c>
@@ -5017,13 +5017,13 @@
         <f>(F73*F74)+F75</f>
         <v>124500</v>
       </c>
-      <c r="G76" s="63"/>
-      <c r="H76" s="63"/>
-      <c r="I76" s="63"/>
-      <c r="J76" s="63"/>
+      <c r="G76" s="62"/>
+      <c r="H76" s="62"/>
+      <c r="I76" s="62"/>
+      <c r="J76" s="62"/>
     </row>
     <row r="77" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A77" s="64"/>
+      <c r="A77" s="58"/>
       <c r="B77" s="13" t="s">
         <v>132</v>
       </c>
@@ -5039,13 +5039,13 @@
       <c r="F77" s="28">
         <v>0.1</v>
       </c>
-      <c r="G77" s="70"/>
-      <c r="H77" s="70"/>
-      <c r="I77" s="70"/>
-      <c r="J77" s="70"/>
+      <c r="G77" s="69"/>
+      <c r="H77" s="69"/>
+      <c r="I77" s="69"/>
+      <c r="J77" s="69"/>
     </row>
     <row r="78" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A78" s="64"/>
+      <c r="A78" s="58"/>
       <c r="B78" s="16" t="s">
         <v>130</v>
       </c>
@@ -5062,43 +5062,43 @@
         <f>F76*(1-F77)</f>
         <v>112050</v>
       </c>
-      <c r="G78" s="58"/>
-      <c r="H78" s="59"/>
-      <c r="I78" s="59"/>
-      <c r="J78" s="60"/>
+      <c r="G78" s="70"/>
+      <c r="H78" s="71"/>
+      <c r="I78" s="71"/>
+      <c r="J78" s="72"/>
     </row>
     <row r="80" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A80" s="64" t="s">
+      <c r="A80" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="B80" s="65" t="s">
+      <c r="B80" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="C80" s="66"/>
-      <c r="D80" s="66"/>
-      <c r="E80" s="66"/>
-      <c r="F80" s="66"/>
-      <c r="G80" s="66"/>
-      <c r="H80" s="66"/>
-      <c r="I80" s="66"/>
-      <c r="J80" s="66"/>
+      <c r="C80" s="64"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="64"/>
+      <c r="H80" s="64"/>
+      <c r="I80" s="64"/>
+      <c r="J80" s="64"/>
     </row>
     <row r="81" spans="1:10" ht="78" customHeight="1">
-      <c r="A81" s="64"/>
-      <c r="B81" s="67" t="s">
+      <c r="A81" s="58"/>
+      <c r="B81" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="C81" s="68"/>
-      <c r="D81" s="68"/>
-      <c r="E81" s="68"/>
-      <c r="F81" s="68"/>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
-      <c r="I81" s="68"/>
-      <c r="J81" s="68"/>
+      <c r="C81" s="60"/>
+      <c r="D81" s="60"/>
+      <c r="E81" s="60"/>
+      <c r="F81" s="60"/>
+      <c r="G81" s="60"/>
+      <c r="H81" s="60"/>
+      <c r="I81" s="60"/>
+      <c r="J81" s="60"/>
     </row>
     <row r="82" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A82" s="64"/>
+      <c r="A82" s="58"/>
       <c r="B82" s="18" t="s">
         <v>33</v>
       </c>
@@ -5114,15 +5114,15 @@
       <c r="F82" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G82" s="69" t="s">
+      <c r="G82" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H82" s="69"/>
-      <c r="I82" s="69"/>
-      <c r="J82" s="69"/>
+      <c r="H82" s="61"/>
+      <c r="I82" s="61"/>
+      <c r="J82" s="61"/>
     </row>
     <row r="83" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A83" s="64"/>
+      <c r="A83" s="58"/>
       <c r="B83" s="13" t="s">
         <v>137</v>
       </c>
@@ -5141,15 +5141,15 @@
         <f>ROUNDUP(D3/2000,0)</f>
         <v>3</v>
       </c>
-      <c r="G83" s="70" t="s">
+      <c r="G83" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="H83" s="70"/>
-      <c r="I83" s="70"/>
-      <c r="J83" s="70"/>
+      <c r="H83" s="69"/>
+      <c r="I83" s="69"/>
+      <c r="J83" s="69"/>
     </row>
     <row r="84" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A84" s="64"/>
+      <c r="A84" s="58"/>
       <c r="B84" s="13" t="s">
         <v>140</v>
       </c>
@@ -5165,15 +5165,15 @@
       <c r="F84" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G84" s="58" t="s">
+      <c r="G84" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="H84" s="59"/>
-      <c r="I84" s="59"/>
-      <c r="J84" s="60"/>
+      <c r="H84" s="71"/>
+      <c r="I84" s="71"/>
+      <c r="J84" s="72"/>
     </row>
     <row r="85" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A85" s="64"/>
+      <c r="A85" s="58"/>
       <c r="B85" s="13" t="s">
         <v>143</v>
       </c>
@@ -5189,15 +5189,15 @@
       <c r="F85" s="23">
         <v>0.05</v>
       </c>
-      <c r="G85" s="58" t="s">
+      <c r="G85" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="H85" s="59"/>
-      <c r="I85" s="59"/>
-      <c r="J85" s="60"/>
+      <c r="H85" s="71"/>
+      <c r="I85" s="71"/>
+      <c r="J85" s="72"/>
     </row>
     <row r="86" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A86" s="64"/>
+      <c r="A86" s="58"/>
       <c r="B86" s="13" t="s">
         <v>146</v>
       </c>
@@ -5216,15 +5216,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$F$12,2,FALSE)</f>
         <v>50280</v>
       </c>
-      <c r="G86" s="63" t="s">
+      <c r="G86" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="H86" s="63"/>
-      <c r="I86" s="63"/>
-      <c r="J86" s="63"/>
+      <c r="H86" s="62"/>
+      <c r="I86" s="62"/>
+      <c r="J86" s="62"/>
     </row>
     <row r="87" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A87" s="64"/>
+      <c r="A87" s="58"/>
       <c r="B87" s="10" t="s">
         <v>148</v>
       </c>
@@ -5243,13 +5243,13 @@
         <f>F83*(F84+F85)*F86</f>
         <v>18100.800000000003</v>
       </c>
-      <c r="G87" s="63"/>
-      <c r="H87" s="63"/>
-      <c r="I87" s="63"/>
-      <c r="J87" s="63"/>
+      <c r="G87" s="62"/>
+      <c r="H87" s="62"/>
+      <c r="I87" s="62"/>
+      <c r="J87" s="62"/>
     </row>
     <row r="88" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A88" s="64"/>
+      <c r="A88" s="58"/>
       <c r="B88" s="13" t="s">
         <v>150</v>
       </c>
@@ -5265,15 +5265,15 @@
       <c r="F88" s="4">
         <v>0.02</v>
       </c>
-      <c r="G88" s="58" t="s">
+      <c r="G88" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="H88" s="59"/>
-      <c r="I88" s="59"/>
-      <c r="J88" s="60"/>
+      <c r="H88" s="71"/>
+      <c r="I88" s="71"/>
+      <c r="J88" s="72"/>
     </row>
     <row r="89" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A89" s="64"/>
+      <c r="A89" s="58"/>
       <c r="B89" s="10" t="s">
         <v>152</v>
       </c>
@@ -5292,13 +5292,13 @@
         <f>F83*(F86)*F88</f>
         <v>3016.8</v>
       </c>
-      <c r="G89" s="63"/>
-      <c r="H89" s="63"/>
-      <c r="I89" s="63"/>
-      <c r="J89" s="63"/>
+      <c r="G89" s="62"/>
+      <c r="H89" s="62"/>
+      <c r="I89" s="62"/>
+      <c r="J89" s="62"/>
     </row>
     <row r="90" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A90" s="64"/>
+      <c r="A90" s="58"/>
       <c r="B90" s="13" t="s">
         <v>154</v>
       </c>
@@ -5317,15 +5317,15 @@
         <f>$J$4*$D$3</f>
         <v>325000</v>
       </c>
-      <c r="G90" s="63" t="s">
+      <c r="G90" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="H90" s="63"/>
-      <c r="I90" s="63"/>
-      <c r="J90" s="63"/>
+      <c r="H90" s="62"/>
+      <c r="I90" s="62"/>
+      <c r="J90" s="62"/>
     </row>
     <row r="91" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A91" s="64"/>
+      <c r="A91" s="58"/>
       <c r="B91" s="13" t="s">
         <v>157</v>
       </c>
@@ -5344,15 +5344,15 @@
         <f t="shared" si="5"/>
         <v>1200</v>
       </c>
-      <c r="G91" s="58" t="s">
+      <c r="G91" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="H91" s="59"/>
-      <c r="I91" s="59"/>
-      <c r="J91" s="60"/>
+      <c r="H91" s="71"/>
+      <c r="I91" s="71"/>
+      <c r="J91" s="72"/>
     </row>
     <row r="92" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A92" s="64"/>
+      <c r="A92" s="58"/>
       <c r="B92" s="13" t="s">
         <v>160</v>
       </c>
@@ -5371,15 +5371,15 @@
         <f>IF($D$5="Yes",$G$4*4500,0)</f>
         <v>9000</v>
       </c>
-      <c r="G92" s="58" t="s">
+      <c r="G92" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="H92" s="59"/>
-      <c r="I92" s="59"/>
-      <c r="J92" s="60"/>
+      <c r="H92" s="71"/>
+      <c r="I92" s="71"/>
+      <c r="J92" s="72"/>
     </row>
     <row r="93" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A93" s="64"/>
+      <c r="A93" s="58"/>
       <c r="B93" s="29" t="s">
         <v>163</v>
       </c>
@@ -5398,25 +5398,25 @@
         <f>SUM(F87,F89:F92)</f>
         <v>356317.6</v>
       </c>
-      <c r="G93" s="58"/>
-      <c r="H93" s="59"/>
-      <c r="I93" s="59"/>
-      <c r="J93" s="60"/>
+      <c r="G93" s="70"/>
+      <c r="H93" s="71"/>
+      <c r="I93" s="71"/>
+      <c r="J93" s="72"/>
     </row>
     <row r="94" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A94" s="64"/>
-      <c r="B94" s="61"/>
-      <c r="C94" s="61"/>
-      <c r="D94" s="61"/>
-      <c r="E94" s="61"/>
-      <c r="F94" s="61"/>
-      <c r="G94" s="61"/>
-      <c r="H94" s="61"/>
-      <c r="I94" s="61"/>
-      <c r="J94" s="61"/>
+      <c r="A94" s="58"/>
+      <c r="B94" s="68"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="68"/>
+      <c r="E94" s="68"/>
+      <c r="F94" s="68"/>
+      <c r="G94" s="68"/>
+      <c r="H94" s="68"/>
+      <c r="I94" s="68"/>
+      <c r="J94" s="68"/>
     </row>
     <row r="95" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A95" s="64"/>
+      <c r="A95" s="58"/>
       <c r="B95" s="13" t="s">
         <v>165</v>
       </c>
@@ -5432,13 +5432,13 @@
       <c r="F95" s="4">
         <v>0.05</v>
       </c>
-      <c r="G95" s="62"/>
-      <c r="H95" s="62"/>
-      <c r="I95" s="62"/>
-      <c r="J95" s="62"/>
+      <c r="G95" s="65"/>
+      <c r="H95" s="65"/>
+      <c r="I95" s="65"/>
+      <c r="J95" s="65"/>
     </row>
     <row r="96" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A96" s="64"/>
+      <c r="A96" s="58"/>
       <c r="B96" s="16"/>
       <c r="C96" s="16"/>
       <c r="D96" s="26">
@@ -5453,13 +5453,79 @@
         <f>F93*(1+F95)</f>
         <v>374133.48</v>
       </c>
-      <c r="G96" s="63"/>
-      <c r="H96" s="63"/>
-      <c r="I96" s="63"/>
-      <c r="J96" s="63"/>
+      <c r="G96" s="62"/>
+      <c r="H96" s="62"/>
+      <c r="I96" s="62"/>
+      <c r="J96" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="G93:J93"/>
+    <mergeCell ref="B94:J94"/>
+    <mergeCell ref="G95:J95"/>
+    <mergeCell ref="G96:J96"/>
+    <mergeCell ref="A80:A96"/>
+    <mergeCell ref="B80:J80"/>
+    <mergeCell ref="B81:J81"/>
+    <mergeCell ref="G82:J82"/>
+    <mergeCell ref="G83:J83"/>
+    <mergeCell ref="G86:J86"/>
+    <mergeCell ref="G87:J87"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="G85:J85"/>
+    <mergeCell ref="G84:J84"/>
+    <mergeCell ref="G91:J91"/>
+    <mergeCell ref="G92:J92"/>
+    <mergeCell ref="G89:J89"/>
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="A70:A78"/>
+    <mergeCell ref="B70:J70"/>
+    <mergeCell ref="B71:J71"/>
+    <mergeCell ref="G72:J72"/>
+    <mergeCell ref="G73:J73"/>
+    <mergeCell ref="G74:J74"/>
+    <mergeCell ref="G76:J76"/>
+    <mergeCell ref="G77:J77"/>
+    <mergeCell ref="G78:J78"/>
+    <mergeCell ref="G75:J75"/>
+    <mergeCell ref="A56:A68"/>
+    <mergeCell ref="B56:J56"/>
+    <mergeCell ref="B57:J57"/>
+    <mergeCell ref="G58:J58"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="G60:J60"/>
+    <mergeCell ref="G61:J61"/>
+    <mergeCell ref="G63:J63"/>
+    <mergeCell ref="G62:J62"/>
+    <mergeCell ref="G64:J64"/>
+    <mergeCell ref="G65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="G67:J67"/>
+    <mergeCell ref="G68:J68"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="G49:J49"/>
+    <mergeCell ref="G50:J50"/>
+    <mergeCell ref="B51:J51"/>
+    <mergeCell ref="A40:A54"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="G45:J45"/>
+    <mergeCell ref="G46:J46"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="G54:J54"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="G33:J33"/>
     <mergeCell ref="A16:A38"/>
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="G18:J18"/>
@@ -5476,72 +5542,6 @@
     <mergeCell ref="G34:J34"/>
     <mergeCell ref="G36:J36"/>
     <mergeCell ref="G37:J37"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="B28:J28"/>
-    <mergeCell ref="B35:J35"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="G49:J49"/>
-    <mergeCell ref="G50:J50"/>
-    <mergeCell ref="B51:J51"/>
-    <mergeCell ref="A40:A54"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="B41:J41"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="G43:J43"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="G45:J45"/>
-    <mergeCell ref="G46:J46"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G54:J54"/>
-    <mergeCell ref="A56:A68"/>
-    <mergeCell ref="B56:J56"/>
-    <mergeCell ref="B57:J57"/>
-    <mergeCell ref="G58:J58"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="G60:J60"/>
-    <mergeCell ref="G61:J61"/>
-    <mergeCell ref="G63:J63"/>
-    <mergeCell ref="G62:J62"/>
-    <mergeCell ref="G64:J64"/>
-    <mergeCell ref="G65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="G67:J67"/>
-    <mergeCell ref="G68:J68"/>
-    <mergeCell ref="G89:J89"/>
-    <mergeCell ref="G90:J90"/>
-    <mergeCell ref="A70:A78"/>
-    <mergeCell ref="B70:J70"/>
-    <mergeCell ref="B71:J71"/>
-    <mergeCell ref="G72:J72"/>
-    <mergeCell ref="G73:J73"/>
-    <mergeCell ref="G74:J74"/>
-    <mergeCell ref="G76:J76"/>
-    <mergeCell ref="G77:J77"/>
-    <mergeCell ref="G78:J78"/>
-    <mergeCell ref="G75:J75"/>
-    <mergeCell ref="G93:J93"/>
-    <mergeCell ref="B94:J94"/>
-    <mergeCell ref="G95:J95"/>
-    <mergeCell ref="G96:J96"/>
-    <mergeCell ref="A80:A96"/>
-    <mergeCell ref="B80:J80"/>
-    <mergeCell ref="B81:J81"/>
-    <mergeCell ref="G82:J82"/>
-    <mergeCell ref="G83:J83"/>
-    <mergeCell ref="G86:J86"/>
-    <mergeCell ref="G87:J87"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="G85:J85"/>
-    <mergeCell ref="G84:J84"/>
-    <mergeCell ref="G91:J91"/>
-    <mergeCell ref="G92:J92"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
@@ -5571,8 +5571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972358DD-1820-401E-852C-2CB83E566002}">
   <dimension ref="A1:S96"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A63" zoomScale="119" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73:J73"/>
+    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="119" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.7" customHeight="1"/>
@@ -5911,37 +5911,37 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="13.7" customHeight="1">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
     </row>
     <row r="17" spans="1:10" ht="45.6" customHeight="1">
-      <c r="A17" s="64"/>
-      <c r="B17" s="67" t="s">
+      <c r="A17" s="58"/>
+      <c r="B17" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
     </row>
     <row r="18" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A18" s="64"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="18" t="s">
         <v>33</v>
       </c>
@@ -5957,15 +5957,15 @@
       <c r="F18" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="69" t="s">
+      <c r="G18" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
     </row>
     <row r="19" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A19" s="64"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="13" t="s">
         <v>36</v>
       </c>
@@ -5984,15 +5984,15 @@
         <f>D19</f>
         <v>4</v>
       </c>
-      <c r="G19" s="63" t="s">
+      <c r="G19" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
     </row>
     <row r="20" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A20" s="64"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="13" t="s">
         <v>39</v>
       </c>
@@ -6008,15 +6008,15 @@
       <c r="F20" s="23">
         <v>0.6</v>
       </c>
-      <c r="G20" s="63" t="s">
+      <c r="G20" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
     </row>
     <row r="21" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A21" s="64"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="13" t="s">
         <v>42</v>
       </c>
@@ -6032,15 +6032,15 @@
       <c r="F21" s="23">
         <v>0.65</v>
       </c>
-      <c r="G21" s="63" t="s">
+      <c r="G21" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="63"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="64"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="19" t="s">
         <v>45</v>
       </c>
@@ -6059,13 +6059,13 @@
         <f>ROUNDUP(F19*F20*F21,0)</f>
         <v>2</v>
       </c>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="64"/>
+      <c r="A23" s="58"/>
       <c r="B23" s="13" t="s">
         <v>47</v>
       </c>
@@ -6081,15 +6081,15 @@
       <c r="F23" s="23">
         <v>0.15</v>
       </c>
-      <c r="G23" s="63" t="s">
+      <c r="G23" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
     </row>
     <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="64"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="13" t="s">
         <v>49</v>
       </c>
@@ -6105,15 +6105,15 @@
       <c r="F24" s="23">
         <v>0.65</v>
       </c>
-      <c r="G24" s="63" t="s">
+      <c r="G24" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
     </row>
     <row r="25" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A25" s="64"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="19" t="s">
         <v>50</v>
       </c>
@@ -6132,13 +6132,13 @@
         <f>ROUNDUP(F19*F23*F24,0)</f>
         <v>1</v>
       </c>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
     </row>
     <row r="26" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A26" s="64"/>
+      <c r="A26" s="58"/>
       <c r="B26" s="13" t="s">
         <v>52</v>
       </c>
@@ -6157,15 +6157,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$F$12,2,FALSE)</f>
         <v>50280</v>
       </c>
-      <c r="G26" s="63" t="s">
+      <c r="G26" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="63"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="63"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
     </row>
     <row r="27" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A27" s="64"/>
+      <c r="A27" s="58"/>
       <c r="B27" s="20" t="s">
         <v>55</v>
       </c>
@@ -6184,27 +6184,27 @@
         <f>(F22+F25)*F26</f>
         <v>150840</v>
       </c>
-      <c r="G27" s="63" t="s">
+      <c r="G27" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
     </row>
     <row r="28" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A28" s="64"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="72"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="66"/>
+      <c r="J28" s="67"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="64"/>
+      <c r="A29" s="58"/>
       <c r="B29" s="13" t="s">
         <v>58</v>
       </c>
@@ -6223,15 +6223,15 @@
         <f>D29</f>
         <v>3</v>
       </c>
-      <c r="G29" s="63" t="s">
+      <c r="G29" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="63"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="63"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="64"/>
+      <c r="A30" s="58"/>
       <c r="B30" s="13" t="s">
         <v>61</v>
       </c>
@@ -6247,15 +6247,15 @@
       <c r="F30" s="23">
         <v>0.33</v>
       </c>
-      <c r="G30" s="63" t="s">
+      <c r="G30" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="63"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="63"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
     </row>
     <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="64"/>
+      <c r="A31" s="58"/>
       <c r="B31" s="13" t="s">
         <v>63</v>
       </c>
@@ -6271,15 +6271,15 @@
       <c r="F31" s="23">
         <v>0.65</v>
       </c>
-      <c r="G31" s="63" t="s">
+      <c r="G31" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
     </row>
     <row r="32" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A32" s="64"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
@@ -6298,13 +6298,13 @@
         <f>ROUNDUP(F29*F30*F31,0)</f>
         <v>1</v>
       </c>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
     </row>
     <row r="33" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A33" s="64"/>
+      <c r="A33" s="58"/>
       <c r="B33" s="13" t="s">
         <v>66</v>
       </c>
@@ -6323,15 +6323,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$G$12,3,FALSE)</f>
         <v>46862</v>
       </c>
-      <c r="G33" s="63" t="s">
+      <c r="G33" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
     </row>
     <row r="34" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A34" s="64"/>
+      <c r="A34" s="58"/>
       <c r="B34" s="16" t="s">
         <v>68</v>
       </c>
@@ -6350,27 +6350,27 @@
         <f>F33*F32</f>
         <v>46862</v>
       </c>
-      <c r="G34" s="63" t="s">
+      <c r="G34" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="63"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="62"/>
     </row>
     <row r="35" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A35" s="64"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="61"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
     </row>
     <row r="36" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A36" s="64"/>
+      <c r="A36" s="58"/>
       <c r="B36" s="13" t="s">
         <v>70</v>
       </c>
@@ -6386,15 +6386,15 @@
       <c r="F36" s="4">
         <v>0.25</v>
       </c>
-      <c r="G36" s="63" t="s">
+      <c r="G36" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="H36" s="63"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="63"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
     </row>
     <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="64"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="13" t="s">
         <v>73</v>
       </c>
@@ -6410,15 +6410,15 @@
       <c r="F37" s="4">
         <v>0.1</v>
       </c>
-      <c r="G37" s="62" t="s">
+      <c r="G37" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="H37" s="62"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="62"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="65"/>
     </row>
     <row r="38" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A38" s="64"/>
+      <c r="A38" s="58"/>
       <c r="B38" s="16" t="s">
         <v>76</v>
       </c>
@@ -6435,43 +6435,43 @@
         <f>(F27+F34)*(1-F36)*(1-F37)</f>
         <v>133448.85</v>
       </c>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
     </row>
     <row r="40" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="65" t="s">
+      <c r="B40" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="66"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="66"/>
-      <c r="I40" s="66"/>
-      <c r="J40" s="66"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="64"/>
+      <c r="J40" s="64"/>
     </row>
     <row r="41" spans="1:10" ht="45" customHeight="1">
-      <c r="A41" s="64"/>
-      <c r="B41" s="67" t="s">
+      <c r="A41" s="58"/>
+      <c r="B41" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="68"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
     </row>
     <row r="42" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A42" s="64"/>
+      <c r="A42" s="58"/>
       <c r="B42" s="18" t="s">
         <v>33</v>
       </c>
@@ -6487,15 +6487,15 @@
       <c r="F42" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="69" t="s">
+      <c r="G42" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H42" s="69"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="69"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="61"/>
     </row>
     <row r="43" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A43" s="64"/>
+      <c r="A43" s="58"/>
       <c r="B43" s="13" t="s">
         <v>79</v>
       </c>
@@ -6514,13 +6514,13 @@
         <f>D3</f>
         <v>5000</v>
       </c>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
     </row>
     <row r="44" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A44" s="64"/>
+      <c r="A44" s="58"/>
       <c r="B44" s="13" t="s">
         <v>81</v>
       </c>
@@ -6539,13 +6539,13 @@
         <f>D4</f>
         <v>0.5</v>
       </c>
-      <c r="G44" s="63"/>
-      <c r="H44" s="63"/>
-      <c r="I44" s="63"/>
-      <c r="J44" s="63"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
     </row>
     <row r="45" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A45" s="64"/>
+      <c r="A45" s="58"/>
       <c r="B45" s="13" t="s">
         <v>83</v>
       </c>
@@ -6561,15 +6561,15 @@
       <c r="F45" s="4">
         <v>0.2</v>
       </c>
-      <c r="G45" s="63" t="s">
+      <c r="G45" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
     </row>
     <row r="46" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A46" s="64"/>
+      <c r="A46" s="58"/>
       <c r="B46" s="10" t="s">
         <v>86</v>
       </c>
@@ -6588,13 +6588,13 @@
         <f>F43*F44*F45</f>
         <v>500</v>
       </c>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="63"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="62"/>
+      <c r="J46" s="62"/>
     </row>
     <row r="47" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A47" s="64"/>
+      <c r="A47" s="58"/>
       <c r="B47" s="13" t="s">
         <v>88</v>
       </c>
@@ -6610,15 +6610,15 @@
       <c r="F47" s="23">
         <v>0.08</v>
       </c>
-      <c r="G47" s="63" t="s">
+      <c r="G47" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="62"/>
     </row>
     <row r="48" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A48" s="64"/>
+      <c r="A48" s="58"/>
       <c r="B48" s="10" t="s">
         <v>90</v>
       </c>
@@ -6637,13 +6637,13 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="G48" s="63"/>
-      <c r="H48" s="63"/>
-      <c r="I48" s="63"/>
-      <c r="J48" s="63"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="62"/>
+      <c r="J48" s="62"/>
     </row>
     <row r="49" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A49" s="64"/>
+      <c r="A49" s="58"/>
       <c r="B49" s="13" t="s">
         <v>92</v>
       </c>
@@ -6662,15 +6662,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$H$12,4,FALSE)</f>
         <v>41000</v>
       </c>
-      <c r="G49" s="63" t="s">
+      <c r="G49" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="H49" s="63"/>
-      <c r="I49" s="63"/>
-      <c r="J49" s="63"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="62"/>
     </row>
     <row r="50" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A50" s="64"/>
+      <c r="A50" s="58"/>
       <c r="B50" s="16" t="s">
         <v>95</v>
       </c>
@@ -6689,27 +6689,27 @@
         <f>F48*F49</f>
         <v>1640000</v>
       </c>
-      <c r="G50" s="63" t="s">
+      <c r="G50" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="H50" s="63"/>
-      <c r="I50" s="63"/>
-      <c r="J50" s="63"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
     </row>
     <row r="51" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A51" s="64"/>
-      <c r="B51" s="71"/>
-      <c r="C51" s="71"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="71"/>
-      <c r="F51" s="71"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="71"/>
-      <c r="I51" s="71"/>
-      <c r="J51" s="72"/>
+      <c r="A51" s="58"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="66"/>
+      <c r="F51" s="66"/>
+      <c r="G51" s="66"/>
+      <c r="H51" s="66"/>
+      <c r="I51" s="66"/>
+      <c r="J51" s="67"/>
     </row>
     <row r="52" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A52" s="64"/>
+      <c r="A52" s="58"/>
       <c r="B52" s="13" t="s">
         <v>97</v>
       </c>
@@ -6725,15 +6725,15 @@
       <c r="F52" s="4">
         <v>0.25</v>
       </c>
-      <c r="G52" s="63" t="s">
+      <c r="G52" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="H52" s="63"/>
-      <c r="I52" s="63"/>
-      <c r="J52" s="63"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="62"/>
+      <c r="J52" s="62"/>
     </row>
     <row r="53" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A53" s="64"/>
+      <c r="A53" s="58"/>
       <c r="B53" s="13" t="s">
         <v>99</v>
       </c>
@@ -6749,15 +6749,15 @@
       <c r="F53" s="4">
         <v>0.1</v>
       </c>
-      <c r="G53" s="62" t="s">
+      <c r="G53" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="H53" s="62"/>
-      <c r="I53" s="62"/>
-      <c r="J53" s="62"/>
+      <c r="H53" s="65"/>
+      <c r="I53" s="65"/>
+      <c r="J53" s="65"/>
     </row>
     <row r="54" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A54" s="64"/>
+      <c r="A54" s="58"/>
       <c r="B54" s="16" t="s">
         <v>100</v>
       </c>
@@ -6774,43 +6774,43 @@
         <f>F50*(1-F52)*(1-F53)</f>
         <v>1107000</v>
       </c>
-      <c r="G54" s="63"/>
-      <c r="H54" s="63"/>
-      <c r="I54" s="63"/>
-      <c r="J54" s="63"/>
+      <c r="G54" s="62"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="62"/>
+      <c r="J54" s="62"/>
     </row>
     <row r="56" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A56" s="64" t="s">
+      <c r="A56" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="65" t="s">
+      <c r="B56" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="66"/>
-      <c r="D56" s="66"/>
-      <c r="E56" s="66"/>
-      <c r="F56" s="66"/>
-      <c r="G56" s="66"/>
-      <c r="H56" s="66"/>
-      <c r="I56" s="66"/>
-      <c r="J56" s="66"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="64"/>
+      <c r="F56" s="64"/>
+      <c r="G56" s="64"/>
+      <c r="H56" s="64"/>
+      <c r="I56" s="64"/>
+      <c r="J56" s="64"/>
     </row>
     <row r="57" spans="1:10" ht="49.35" customHeight="1">
-      <c r="A57" s="64"/>
-      <c r="B57" s="67" t="s">
+      <c r="A57" s="58"/>
+      <c r="B57" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="68"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="68"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="68"/>
-      <c r="H57" s="68"/>
-      <c r="I57" s="68"/>
-      <c r="J57" s="68"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="60"/>
+      <c r="I57" s="60"/>
+      <c r="J57" s="60"/>
     </row>
     <row r="58" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A58" s="64"/>
+      <c r="A58" s="58"/>
       <c r="B58" s="18" t="s">
         <v>33</v>
       </c>
@@ -6826,15 +6826,15 @@
       <c r="F58" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G58" s="69" t="s">
+      <c r="G58" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H58" s="69"/>
-      <c r="I58" s="69"/>
-      <c r="J58" s="69"/>
+      <c r="H58" s="61"/>
+      <c r="I58" s="61"/>
+      <c r="J58" s="61"/>
     </row>
     <row r="59" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A59" s="64"/>
+      <c r="A59" s="58"/>
       <c r="B59" s="13" t="s">
         <v>103</v>
       </c>
@@ -6852,15 +6852,15 @@
         <f>D59</f>
         <v>3.2</v>
       </c>
-      <c r="G59" s="63" t="s">
+      <c r="G59" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="H59" s="63"/>
-      <c r="I59" s="63"/>
-      <c r="J59" s="63"/>
+      <c r="H59" s="62"/>
+      <c r="I59" s="62"/>
+      <c r="J59" s="62"/>
     </row>
     <row r="60" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A60" s="64"/>
+      <c r="A60" s="58"/>
       <c r="B60" s="13" t="s">
         <v>106</v>
       </c>
@@ -6879,13 +6879,13 @@
         <f>E60</f>
         <v>5000</v>
       </c>
-      <c r="G60" s="63"/>
-      <c r="H60" s="63"/>
-      <c r="I60" s="63"/>
-      <c r="J60" s="63"/>
+      <c r="G60" s="62"/>
+      <c r="H60" s="62"/>
+      <c r="I60" s="62"/>
+      <c r="J60" s="62"/>
     </row>
     <row r="61" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A61" s="64"/>
+      <c r="A61" s="58"/>
       <c r="B61" s="13" t="s">
         <v>107</v>
       </c>
@@ -6904,13 +6904,13 @@
         <f>E61</f>
         <v>0.5</v>
       </c>
-      <c r="G61" s="63"/>
-      <c r="H61" s="63"/>
-      <c r="I61" s="63"/>
-      <c r="J61" s="63"/>
+      <c r="G61" s="62"/>
+      <c r="H61" s="62"/>
+      <c r="I61" s="62"/>
+      <c r="J61" s="62"/>
     </row>
     <row r="62" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A62" s="64"/>
+      <c r="A62" s="58"/>
       <c r="B62" s="13" t="s">
         <v>108</v>
       </c>
@@ -6926,15 +6926,15 @@
       <c r="F62" s="5">
         <v>53</v>
       </c>
-      <c r="G62" s="70" t="s">
+      <c r="G62" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="H62" s="70"/>
-      <c r="I62" s="70"/>
-      <c r="J62" s="70"/>
+      <c r="H62" s="69"/>
+      <c r="I62" s="69"/>
+      <c r="J62" s="69"/>
     </row>
     <row r="63" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A63" s="64"/>
+      <c r="A63" s="58"/>
       <c r="B63" s="10" t="s">
         <v>111</v>
       </c>
@@ -6953,13 +6953,13 @@
         <f>F59*F60*F61*F62</f>
         <v>424000</v>
       </c>
-      <c r="G63" s="63"/>
-      <c r="H63" s="63"/>
-      <c r="I63" s="63"/>
-      <c r="J63" s="63"/>
+      <c r="G63" s="62"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="62"/>
+      <c r="J63" s="62"/>
     </row>
     <row r="64" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A64" s="64"/>
+      <c r="A64" s="58"/>
       <c r="B64" s="13" t="s">
         <v>113</v>
       </c>
@@ -6975,15 +6975,15 @@
       <c r="F64" s="4">
         <v>0.75</v>
       </c>
-      <c r="G64" s="63" t="s">
+      <c r="G64" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H64" s="63"/>
-      <c r="I64" s="63"/>
-      <c r="J64" s="63"/>
+      <c r="H64" s="62"/>
+      <c r="I64" s="62"/>
+      <c r="J64" s="62"/>
     </row>
     <row r="65" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A65" s="64"/>
+      <c r="A65" s="58"/>
       <c r="B65" s="16" t="s">
         <v>115</v>
       </c>
@@ -7002,25 +7002,25 @@
         <f t="shared" si="4"/>
         <v>318000</v>
       </c>
-      <c r="G65" s="58"/>
-      <c r="H65" s="59"/>
-      <c r="I65" s="59"/>
-      <c r="J65" s="60"/>
+      <c r="G65" s="70"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71"/>
+      <c r="J65" s="72"/>
     </row>
     <row r="66" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A66" s="64"/>
-      <c r="B66" s="61"/>
-      <c r="C66" s="61"/>
-      <c r="D66" s="61"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="61"/>
-      <c r="G66" s="61"/>
-      <c r="H66" s="61"/>
-      <c r="I66" s="61"/>
-      <c r="J66" s="61"/>
+      <c r="A66" s="58"/>
+      <c r="B66" s="68"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="68"/>
+      <c r="H66" s="68"/>
+      <c r="I66" s="68"/>
+      <c r="J66" s="68"/>
     </row>
     <row r="67" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A67" s="64"/>
+      <c r="A67" s="58"/>
       <c r="B67" s="13" t="s">
         <v>117</v>
       </c>
@@ -7036,15 +7036,15 @@
       <c r="F67" s="4">
         <v>0.25</v>
       </c>
-      <c r="G67" s="62" t="s">
+      <c r="G67" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="H67" s="62"/>
-      <c r="I67" s="62"/>
-      <c r="J67" s="62"/>
+      <c r="H67" s="65"/>
+      <c r="I67" s="65"/>
+      <c r="J67" s="65"/>
     </row>
     <row r="68" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A68" s="64"/>
+      <c r="A68" s="58"/>
       <c r="B68" s="16" t="s">
         <v>118</v>
       </c>
@@ -7061,43 +7061,43 @@
         <f>F65*(1-F67)</f>
         <v>238500</v>
       </c>
-      <c r="G68" s="63"/>
-      <c r="H68" s="63"/>
-      <c r="I68" s="63"/>
-      <c r="J68" s="63"/>
+      <c r="G68" s="62"/>
+      <c r="H68" s="62"/>
+      <c r="I68" s="62"/>
+      <c r="J68" s="62"/>
     </row>
     <row r="70" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A70" s="64" t="s">
+      <c r="A70" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="B70" s="65" t="s">
+      <c r="B70" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="C70" s="66"/>
-      <c r="D70" s="66"/>
-      <c r="E70" s="66"/>
-      <c r="F70" s="66"/>
-      <c r="G70" s="66"/>
-      <c r="H70" s="66"/>
-      <c r="I70" s="66"/>
-      <c r="J70" s="66"/>
+      <c r="C70" s="64"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="64"/>
+      <c r="F70" s="64"/>
+      <c r="G70" s="64"/>
+      <c r="H70" s="64"/>
+      <c r="I70" s="64"/>
+      <c r="J70" s="64"/>
     </row>
     <row r="71" spans="1:10" ht="41.45" customHeight="1">
-      <c r="A71" s="64"/>
-      <c r="B71" s="67" t="s">
+      <c r="A71" s="58"/>
+      <c r="B71" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="C71" s="68"/>
-      <c r="D71" s="68"/>
-      <c r="E71" s="68"/>
-      <c r="F71" s="68"/>
-      <c r="G71" s="68"/>
-      <c r="H71" s="68"/>
-      <c r="I71" s="68"/>
-      <c r="J71" s="68"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="60"/>
+      <c r="F71" s="60"/>
+      <c r="G71" s="60"/>
+      <c r="H71" s="60"/>
+      <c r="I71" s="60"/>
+      <c r="J71" s="60"/>
     </row>
     <row r="72" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A72" s="64"/>
+      <c r="A72" s="58"/>
       <c r="B72" s="18" t="s">
         <v>33</v>
       </c>
@@ -7113,15 +7113,15 @@
       <c r="F72" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G72" s="69" t="s">
+      <c r="G72" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H72" s="69"/>
-      <c r="I72" s="69"/>
-      <c r="J72" s="69"/>
+      <c r="H72" s="61"/>
+      <c r="I72" s="61"/>
+      <c r="J72" s="61"/>
     </row>
     <row r="73" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A73" s="64"/>
+      <c r="A73" s="58"/>
       <c r="B73" s="13" t="s">
         <v>121</v>
       </c>
@@ -7140,15 +7140,15 @@
         <f>E73</f>
         <v>175000</v>
       </c>
-      <c r="G73" s="70" t="s">
+      <c r="G73" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="H73" s="70"/>
-      <c r="I73" s="70"/>
-      <c r="J73" s="70"/>
+      <c r="H73" s="69"/>
+      <c r="I73" s="69"/>
+      <c r="J73" s="69"/>
     </row>
     <row r="74" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A74" s="64"/>
+      <c r="A74" s="58"/>
       <c r="B74" s="13" t="s">
         <v>124</v>
       </c>
@@ -7164,15 +7164,15 @@
       <c r="F74" s="28">
         <v>0.3</v>
       </c>
-      <c r="G74" s="63" t="s">
+      <c r="G74" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="H74" s="63"/>
-      <c r="I74" s="63"/>
-      <c r="J74" s="63"/>
+      <c r="H74" s="62"/>
+      <c r="I74" s="62"/>
+      <c r="J74" s="62"/>
     </row>
     <row r="75" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A75" s="64"/>
+      <c r="A75" s="58"/>
       <c r="B75" s="13" t="s">
         <v>127</v>
       </c>
@@ -7191,15 +7191,15 @@
         <f>IF($D$5="Yes",$G$4*36000,0)</f>
         <v>72000</v>
       </c>
-      <c r="G75" s="63" t="s">
+      <c r="G75" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="H75" s="63"/>
-      <c r="I75" s="63"/>
-      <c r="J75" s="63"/>
+      <c r="H75" s="62"/>
+      <c r="I75" s="62"/>
+      <c r="J75" s="62"/>
     </row>
     <row r="76" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A76" s="64"/>
+      <c r="A76" s="58"/>
       <c r="B76" s="13" t="s">
         <v>130</v>
       </c>
@@ -7218,13 +7218,13 @@
         <f>(F73*F74)+F75</f>
         <v>124500</v>
       </c>
-      <c r="G76" s="63"/>
-      <c r="H76" s="63"/>
-      <c r="I76" s="63"/>
-      <c r="J76" s="63"/>
+      <c r="G76" s="62"/>
+      <c r="H76" s="62"/>
+      <c r="I76" s="62"/>
+      <c r="J76" s="62"/>
     </row>
     <row r="77" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A77" s="64"/>
+      <c r="A77" s="58"/>
       <c r="B77" s="13" t="s">
         <v>132</v>
       </c>
@@ -7240,13 +7240,13 @@
       <c r="F77" s="28">
         <v>0.1</v>
       </c>
-      <c r="G77" s="70"/>
-      <c r="H77" s="70"/>
-      <c r="I77" s="70"/>
-      <c r="J77" s="70"/>
+      <c r="G77" s="69"/>
+      <c r="H77" s="69"/>
+      <c r="I77" s="69"/>
+      <c r="J77" s="69"/>
     </row>
     <row r="78" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A78" s="64"/>
+      <c r="A78" s="58"/>
       <c r="B78" s="16" t="s">
         <v>130</v>
       </c>
@@ -7263,43 +7263,43 @@
         <f>F76*(1-F77)</f>
         <v>112050</v>
       </c>
-      <c r="G78" s="58"/>
-      <c r="H78" s="59"/>
-      <c r="I78" s="59"/>
-      <c r="J78" s="60"/>
+      <c r="G78" s="70"/>
+      <c r="H78" s="71"/>
+      <c r="I78" s="71"/>
+      <c r="J78" s="72"/>
     </row>
     <row r="80" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A80" s="64" t="s">
+      <c r="A80" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="B80" s="65" t="s">
+      <c r="B80" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="C80" s="66"/>
-      <c r="D80" s="66"/>
-      <c r="E80" s="66"/>
-      <c r="F80" s="66"/>
-      <c r="G80" s="66"/>
-      <c r="H80" s="66"/>
-      <c r="I80" s="66"/>
-      <c r="J80" s="66"/>
+      <c r="C80" s="64"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="64"/>
+      <c r="H80" s="64"/>
+      <c r="I80" s="64"/>
+      <c r="J80" s="64"/>
     </row>
     <row r="81" spans="1:10" ht="78" customHeight="1">
-      <c r="A81" s="64"/>
-      <c r="B81" s="67" t="s">
+      <c r="A81" s="58"/>
+      <c r="B81" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="C81" s="68"/>
-      <c r="D81" s="68"/>
-      <c r="E81" s="68"/>
-      <c r="F81" s="68"/>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
-      <c r="I81" s="68"/>
-      <c r="J81" s="68"/>
+      <c r="C81" s="60"/>
+      <c r="D81" s="60"/>
+      <c r="E81" s="60"/>
+      <c r="F81" s="60"/>
+      <c r="G81" s="60"/>
+      <c r="H81" s="60"/>
+      <c r="I81" s="60"/>
+      <c r="J81" s="60"/>
     </row>
     <row r="82" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A82" s="64"/>
+      <c r="A82" s="58"/>
       <c r="B82" s="18" t="s">
         <v>33</v>
       </c>
@@ -7315,15 +7315,15 @@
       <c r="F82" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G82" s="69" t="s">
+      <c r="G82" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="H82" s="69"/>
-      <c r="I82" s="69"/>
-      <c r="J82" s="69"/>
+      <c r="H82" s="61"/>
+      <c r="I82" s="61"/>
+      <c r="J82" s="61"/>
     </row>
     <row r="83" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A83" s="64"/>
+      <c r="A83" s="58"/>
       <c r="B83" s="13" t="s">
         <v>137</v>
       </c>
@@ -7342,15 +7342,15 @@
         <f>ROUNDUP(D3/2000,0)</f>
         <v>3</v>
       </c>
-      <c r="G83" s="70" t="s">
+      <c r="G83" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="H83" s="70"/>
-      <c r="I83" s="70"/>
-      <c r="J83" s="70"/>
+      <c r="H83" s="69"/>
+      <c r="I83" s="69"/>
+      <c r="J83" s="69"/>
     </row>
     <row r="84" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A84" s="64"/>
+      <c r="A84" s="58"/>
       <c r="B84" s="13" t="s">
         <v>140</v>
       </c>
@@ -7366,15 +7366,15 @@
       <c r="F84" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G84" s="58" t="s">
+      <c r="G84" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="H84" s="59"/>
-      <c r="I84" s="59"/>
-      <c r="J84" s="60"/>
+      <c r="H84" s="71"/>
+      <c r="I84" s="71"/>
+      <c r="J84" s="72"/>
     </row>
     <row r="85" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A85" s="64"/>
+      <c r="A85" s="58"/>
       <c r="B85" s="13" t="s">
         <v>143</v>
       </c>
@@ -7390,15 +7390,15 @@
       <c r="F85" s="23">
         <v>0.05</v>
       </c>
-      <c r="G85" s="58" t="s">
+      <c r="G85" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="H85" s="59"/>
-      <c r="I85" s="59"/>
-      <c r="J85" s="60"/>
+      <c r="H85" s="71"/>
+      <c r="I85" s="71"/>
+      <c r="J85" s="72"/>
     </row>
     <row r="86" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A86" s="64"/>
+      <c r="A86" s="58"/>
       <c r="B86" s="13" t="s">
         <v>146</v>
       </c>
@@ -7417,15 +7417,15 @@
         <f>VLOOKUP($J$3,Lists!$E$3:$F$12,2,FALSE)</f>
         <v>50280</v>
       </c>
-      <c r="G86" s="63" t="s">
+      <c r="G86" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="H86" s="63"/>
-      <c r="I86" s="63"/>
-      <c r="J86" s="63"/>
+      <c r="H86" s="62"/>
+      <c r="I86" s="62"/>
+      <c r="J86" s="62"/>
     </row>
     <row r="87" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A87" s="64"/>
+      <c r="A87" s="58"/>
       <c r="B87" s="10" t="s">
         <v>148</v>
       </c>
@@ -7444,13 +7444,13 @@
         <f>F83*(F84+F85)*F86</f>
         <v>18100.800000000003</v>
       </c>
-      <c r="G87" s="63"/>
-      <c r="H87" s="63"/>
-      <c r="I87" s="63"/>
-      <c r="J87" s="63"/>
+      <c r="G87" s="62"/>
+      <c r="H87" s="62"/>
+      <c r="I87" s="62"/>
+      <c r="J87" s="62"/>
     </row>
     <row r="88" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A88" s="64"/>
+      <c r="A88" s="58"/>
       <c r="B88" s="13" t="s">
         <v>150</v>
       </c>
@@ -7466,15 +7466,15 @@
       <c r="F88" s="4">
         <v>0.02</v>
       </c>
-      <c r="G88" s="58" t="s">
+      <c r="G88" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="H88" s="59"/>
-      <c r="I88" s="59"/>
-      <c r="J88" s="60"/>
+      <c r="H88" s="71"/>
+      <c r="I88" s="71"/>
+      <c r="J88" s="72"/>
     </row>
     <row r="89" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A89" s="64"/>
+      <c r="A89" s="58"/>
       <c r="B89" s="10" t="s">
         <v>152</v>
       </c>
@@ -7493,13 +7493,13 @@
         <f>F83*(F86)*F88</f>
         <v>3016.8</v>
       </c>
-      <c r="G89" s="63"/>
-      <c r="H89" s="63"/>
-      <c r="I89" s="63"/>
-      <c r="J89" s="63"/>
+      <c r="G89" s="62"/>
+      <c r="H89" s="62"/>
+      <c r="I89" s="62"/>
+      <c r="J89" s="62"/>
     </row>
     <row r="90" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A90" s="64"/>
+      <c r="A90" s="58"/>
       <c r="B90" s="13" t="s">
         <v>154</v>
       </c>
@@ -7518,15 +7518,15 @@
         <f>$J$4*$D$3</f>
         <v>325000</v>
       </c>
-      <c r="G90" s="63" t="s">
+      <c r="G90" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="H90" s="63"/>
-      <c r="I90" s="63"/>
-      <c r="J90" s="63"/>
+      <c r="H90" s="62"/>
+      <c r="I90" s="62"/>
+      <c r="J90" s="62"/>
     </row>
     <row r="91" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A91" s="64"/>
+      <c r="A91" s="58"/>
       <c r="B91" s="13" t="s">
         <v>157</v>
       </c>
@@ -7545,15 +7545,15 @@
         <f t="shared" si="5"/>
         <v>1200</v>
       </c>
-      <c r="G91" s="58" t="s">
+      <c r="G91" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="H91" s="59"/>
-      <c r="I91" s="59"/>
-      <c r="J91" s="60"/>
+      <c r="H91" s="71"/>
+      <c r="I91" s="71"/>
+      <c r="J91" s="72"/>
     </row>
     <row r="92" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A92" s="64"/>
+      <c r="A92" s="58"/>
       <c r="B92" s="13" t="s">
         <v>160</v>
       </c>
@@ -7572,15 +7572,15 @@
         <f>IF($D$5="Yes",$G$4*4500,0)</f>
         <v>9000</v>
       </c>
-      <c r="G92" s="58" t="s">
+      <c r="G92" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="H92" s="59"/>
-      <c r="I92" s="59"/>
-      <c r="J92" s="60"/>
+      <c r="H92" s="71"/>
+      <c r="I92" s="71"/>
+      <c r="J92" s="72"/>
     </row>
     <row r="93" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A93" s="64"/>
+      <c r="A93" s="58"/>
       <c r="B93" s="29" t="s">
         <v>163</v>
       </c>
@@ -7599,25 +7599,25 @@
         <f>SUM(F87,F89:F92)</f>
         <v>356317.6</v>
       </c>
-      <c r="G93" s="58"/>
-      <c r="H93" s="59"/>
-      <c r="I93" s="59"/>
-      <c r="J93" s="60"/>
+      <c r="G93" s="70"/>
+      <c r="H93" s="71"/>
+      <c r="I93" s="71"/>
+      <c r="J93" s="72"/>
     </row>
     <row r="94" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A94" s="64"/>
-      <c r="B94" s="61"/>
-      <c r="C94" s="61"/>
-      <c r="D94" s="61"/>
-      <c r="E94" s="61"/>
-      <c r="F94" s="61"/>
-      <c r="G94" s="61"/>
-      <c r="H94" s="61"/>
-      <c r="I94" s="61"/>
-      <c r="J94" s="61"/>
+      <c r="A94" s="58"/>
+      <c r="B94" s="68"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="68"/>
+      <c r="E94" s="68"/>
+      <c r="F94" s="68"/>
+      <c r="G94" s="68"/>
+      <c r="H94" s="68"/>
+      <c r="I94" s="68"/>
+      <c r="J94" s="68"/>
     </row>
     <row r="95" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A95" s="64"/>
+      <c r="A95" s="58"/>
       <c r="B95" s="13" t="s">
         <v>165</v>
       </c>
@@ -7633,13 +7633,13 @@
       <c r="F95" s="4">
         <v>0.05</v>
       </c>
-      <c r="G95" s="62"/>
-      <c r="H95" s="62"/>
-      <c r="I95" s="62"/>
-      <c r="J95" s="62"/>
+      <c r="G95" s="65"/>
+      <c r="H95" s="65"/>
+      <c r="I95" s="65"/>
+      <c r="J95" s="65"/>
     </row>
     <row r="96" spans="1:10" ht="13.7" customHeight="1">
-      <c r="A96" s="64"/>
+      <c r="A96" s="58"/>
       <c r="B96" s="16"/>
       <c r="C96" s="16"/>
       <c r="D96" s="26">
@@ -7654,30 +7654,62 @@
         <f>F93*(1+F95)</f>
         <v>374133.48</v>
       </c>
-      <c r="G96" s="63"/>
-      <c r="H96" s="63"/>
-      <c r="I96" s="63"/>
-      <c r="J96" s="63"/>
+      <c r="G96" s="62"/>
+      <c r="H96" s="62"/>
+      <c r="I96" s="62"/>
+      <c r="J96" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="B28:J28"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="G93:J93"/>
+    <mergeCell ref="B94:J94"/>
+    <mergeCell ref="A80:A96"/>
+    <mergeCell ref="B80:J80"/>
+    <mergeCell ref="B81:J81"/>
+    <mergeCell ref="G82:J82"/>
+    <mergeCell ref="G83:J83"/>
+    <mergeCell ref="G84:J84"/>
+    <mergeCell ref="G85:J85"/>
+    <mergeCell ref="G86:J86"/>
+    <mergeCell ref="G87:J87"/>
+    <mergeCell ref="G88:J88"/>
+    <mergeCell ref="G95:J95"/>
+    <mergeCell ref="G96:J96"/>
+    <mergeCell ref="G89:J89"/>
+    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="G91:J91"/>
+    <mergeCell ref="G92:J92"/>
+    <mergeCell ref="A70:A78"/>
+    <mergeCell ref="B70:J70"/>
+    <mergeCell ref="B71:J71"/>
+    <mergeCell ref="G72:J72"/>
+    <mergeCell ref="G73:J73"/>
+    <mergeCell ref="G74:J74"/>
+    <mergeCell ref="G75:J75"/>
+    <mergeCell ref="G76:J76"/>
+    <mergeCell ref="G77:J77"/>
+    <mergeCell ref="G78:J78"/>
+    <mergeCell ref="G68:J68"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="G54:J54"/>
+    <mergeCell ref="A56:A68"/>
+    <mergeCell ref="B56:J56"/>
+    <mergeCell ref="B57:J57"/>
+    <mergeCell ref="G58:J58"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="G60:J60"/>
+    <mergeCell ref="G61:J61"/>
+    <mergeCell ref="G62:J62"/>
+    <mergeCell ref="G63:J63"/>
+    <mergeCell ref="G64:J64"/>
+    <mergeCell ref="G65:J65"/>
+    <mergeCell ref="B66:J66"/>
+    <mergeCell ref="G67:J67"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="G49:J49"/>
+    <mergeCell ref="G50:J50"/>
+    <mergeCell ref="B51:J51"/>
     <mergeCell ref="G52:J52"/>
     <mergeCell ref="G37:J37"/>
     <mergeCell ref="G38:J38"/>
@@ -7694,55 +7726,23 @@
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="G49:J49"/>
-    <mergeCell ref="G50:J50"/>
-    <mergeCell ref="B51:J51"/>
-    <mergeCell ref="G68:J68"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G54:J54"/>
-    <mergeCell ref="A56:A68"/>
-    <mergeCell ref="B56:J56"/>
-    <mergeCell ref="B57:J57"/>
-    <mergeCell ref="G58:J58"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="G60:J60"/>
-    <mergeCell ref="G61:J61"/>
-    <mergeCell ref="G62:J62"/>
-    <mergeCell ref="G63:J63"/>
-    <mergeCell ref="G64:J64"/>
-    <mergeCell ref="G65:J65"/>
-    <mergeCell ref="B66:J66"/>
-    <mergeCell ref="G67:J67"/>
-    <mergeCell ref="G91:J91"/>
-    <mergeCell ref="G92:J92"/>
-    <mergeCell ref="A70:A78"/>
-    <mergeCell ref="B70:J70"/>
-    <mergeCell ref="B71:J71"/>
-    <mergeCell ref="G72:J72"/>
-    <mergeCell ref="G73:J73"/>
-    <mergeCell ref="G74:J74"/>
-    <mergeCell ref="G75:J75"/>
-    <mergeCell ref="G76:J76"/>
-    <mergeCell ref="G77:J77"/>
-    <mergeCell ref="G78:J78"/>
-    <mergeCell ref="G93:J93"/>
-    <mergeCell ref="B94:J94"/>
-    <mergeCell ref="A80:A96"/>
-    <mergeCell ref="B80:J80"/>
-    <mergeCell ref="B81:J81"/>
-    <mergeCell ref="G82:J82"/>
-    <mergeCell ref="G83:J83"/>
-    <mergeCell ref="G84:J84"/>
-    <mergeCell ref="G85:J85"/>
-    <mergeCell ref="G86:J86"/>
-    <mergeCell ref="G87:J87"/>
-    <mergeCell ref="G88:J88"/>
-    <mergeCell ref="G95:J95"/>
-    <mergeCell ref="G96:J96"/>
-    <mergeCell ref="G89:J89"/>
-    <mergeCell ref="G90:J90"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
@@ -7772,8 +7772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9F39E0-A2D0-4352-951C-B83BA4C81993}">
   <dimension ref="E2:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:H43"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8268,8 +8268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB613458-C399-4236-80B2-A648D5D4F436}">
   <dimension ref="E2:K12"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>